<commit_message>
fixed db connection issue
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC186B4E-A179-4911-850D-0A97A5A45B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5160B0B3-1EED-46E3-AE79-76558A8764A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
@@ -898,7 +898,7 @@
   <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,7 +983,7 @@
         <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1040,7 +1040,7 @@
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
@@ -1086,7 +1086,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
@@ -1132,7 +1132,7 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
@@ -1175,7 +1175,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -1215,7 +1215,7 @@
         <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
cleared all sync issues
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5160B0B3-1EED-46E3-AE79-76558A8764A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2D8FA-3822-46C6-AD03-C20FF5608EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Registration" sheetId="1" r:id="rId2"/>
     <sheet name="Login" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Registration!$A$1:$T$69</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -182,9 +185,6 @@
     <t>Password should contain at least one lower case letter</t>
   </si>
   <si>
-    <t>Password should contain at least one non alpha numeric character</t>
-  </si>
-  <si>
     <t>Password should contain at least one number</t>
   </si>
   <si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>sdgsgewsd</t>
+  </si>
+  <si>
+    <t>Password should contain at least one non-alphanumeric character</t>
   </si>
 </sst>
 </file>
@@ -844,47 +847,47 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -897,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38982D-3F95-4179-9809-2B80AF189016}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -977,16 +980,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1034,16 +1037,16 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -1080,16 +1083,16 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1126,16 +1129,16 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -1169,16 +1172,16 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -1204,21 +1207,21 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1244,21 +1247,21 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1286,21 +1289,21 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1331,16 +1334,16 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1371,16 +1374,16 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1411,16 +1414,16 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1451,16 +1454,16 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1490,16 +1493,16 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1525,21 +1528,21 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1565,21 +1568,21 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1610,16 +1613,16 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1650,16 +1653,16 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
@@ -1688,16 +1691,16 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1726,16 +1729,16 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1763,21 +1766,21 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1806,16 +1809,16 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
         <v>32</v>
@@ -1841,21 +1844,21 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1881,21 +1884,21 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1923,21 +1926,21 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -1968,16 +1971,16 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -2008,16 +2011,16 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -2048,16 +2051,16 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -2088,16 +2091,16 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2127,16 +2130,16 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2162,21 +2165,21 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2202,21 +2205,21 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2247,16 +2250,16 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2287,16 +2290,16 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
@@ -2325,16 +2328,16 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2363,16 +2366,16 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -2400,21 +2403,21 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2443,16 +2446,16 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E38" t="s">
         <v>32</v>
@@ -2478,21 +2481,21 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2518,21 +2521,21 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2560,21 +2563,21 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2605,16 +2608,16 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2645,16 +2648,16 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2685,16 +2688,16 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2725,16 +2728,16 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2764,16 +2767,16 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -2799,21 +2802,21 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2839,21 +2842,21 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
       <c r="T47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2884,16 +2887,16 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2924,16 +2927,16 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" t="s">
@@ -2962,16 +2965,16 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -3000,16 +3003,16 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -3037,21 +3040,21 @@
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -3080,16 +3083,16 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E54" t="s">
         <v>32</v>
@@ -3115,21 +3118,21 @@
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -3155,21 +3158,21 @@
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -3197,21 +3200,21 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -3242,16 +3245,16 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -3282,16 +3285,16 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
@@ -3322,16 +3325,16 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -3362,16 +3365,16 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -3401,16 +3404,16 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -3436,21 +3439,21 @@
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
@@ -3476,21 +3479,21 @@
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -3521,16 +3524,16 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
@@ -3561,16 +3564,16 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" t="s">
@@ -3599,16 +3602,16 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
@@ -3637,16 +3640,16 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
@@ -3674,21 +3677,21 @@
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E69" t="s">
         <v>12</v>
@@ -3776,13 +3779,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -3793,19 +3796,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -3813,19 +3816,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -3833,16 +3836,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -3850,39 +3853,39 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" t="s">
         <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F6" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed unwanted lib in register
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2D8FA-3822-46C6-AD03-C20FF5608EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D54F30-5EB6-4176-BD85-DE3DC8D78A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
@@ -901,7 +901,7 @@
   <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,7 +1178,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>56</v>
@@ -1218,7 +1218,7 @@
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
@@ -1258,7 +1258,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
@@ -1300,7 +1300,7 @@
         <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>56</v>
@@ -1340,7 +1340,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>56</v>
@@ -1380,7 +1380,7 @@
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>56</v>
@@ -1420,7 +1420,7 @@
         <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
         <v>56</v>
@@ -1460,7 +1460,7 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>56</v>
@@ -1499,7 +1499,7 @@
         <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
         <v>56</v>
@@ -1539,7 +1539,7 @@
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
@@ -1579,7 +1579,7 @@
         <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>56</v>
@@ -1619,7 +1619,7 @@
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -1659,7 +1659,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
@@ -1697,7 +1697,7 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
@@ -1735,7 +1735,7 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
@@ -1777,7 +1777,7 @@
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
@@ -1815,7 +1815,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
         <v>56</v>
@@ -1855,7 +1855,7 @@
         <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
@@ -1895,7 +1895,7 @@
         <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
         <v>56</v>
@@ -1937,7 +1937,7 @@
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
         <v>56</v>
@@ -1977,7 +1977,7 @@
         <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
         <v>56</v>
@@ -2017,7 +2017,7 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
         <v>56</v>
@@ -2057,7 +2057,7 @@
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
         <v>56</v>
@@ -2097,7 +2097,7 @@
         <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -2136,7 +2136,7 @@
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
         <v>56</v>
@@ -2176,7 +2176,7 @@
         <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
         <v>56</v>
@@ -2216,7 +2216,7 @@
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
         <v>56</v>
@@ -2256,7 +2256,7 @@
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -2296,7 +2296,7 @@
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
         <v>56</v>
@@ -2334,7 +2334,7 @@
         <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
         <v>56</v>
@@ -2372,7 +2372,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
         <v>56</v>
@@ -2414,7 +2414,7 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>56</v>
@@ -2452,7 +2452,7 @@
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
         <v>56</v>
@@ -2492,7 +2492,7 @@
         <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
         <v>56</v>
@@ -2532,7 +2532,7 @@
         <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
         <v>56</v>
@@ -2574,7 +2574,7 @@
         <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
         <v>56</v>
@@ -2614,7 +2614,7 @@
         <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
         <v>56</v>
@@ -2654,7 +2654,7 @@
         <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
         <v>56</v>
@@ -2694,7 +2694,7 @@
         <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s">
         <v>56</v>
@@ -2734,7 +2734,7 @@
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
         <v>56</v>
@@ -2773,7 +2773,7 @@
         <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
         <v>56</v>
@@ -2813,7 +2813,7 @@
         <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
         <v>56</v>
@@ -2853,7 +2853,7 @@
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D48" t="s">
         <v>56</v>
@@ -2893,7 +2893,7 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D49" t="s">
         <v>56</v>
@@ -2933,7 +2933,7 @@
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s">
         <v>56</v>
@@ -2971,7 +2971,7 @@
         <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
         <v>56</v>
@@ -3009,7 +3009,7 @@
         <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D52" t="s">
         <v>56</v>
@@ -3051,7 +3051,7 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s">
         <v>56</v>
@@ -3089,7 +3089,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -3129,7 +3129,7 @@
         <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
         <v>56</v>
@@ -3169,7 +3169,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D56" t="s">
         <v>56</v>
@@ -3211,7 +3211,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D57" t="s">
         <v>56</v>
@@ -3251,7 +3251,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D58" t="s">
         <v>56</v>
@@ -3291,7 +3291,7 @@
         <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D59" t="s">
         <v>56</v>
@@ -3331,7 +3331,7 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D60" t="s">
         <v>56</v>
@@ -3371,7 +3371,7 @@
         <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D61" t="s">
         <v>56</v>
@@ -3410,7 +3410,7 @@
         <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D62" t="s">
         <v>56</v>
@@ -3450,7 +3450,7 @@
         <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D63" t="s">
         <v>56</v>
@@ -3490,7 +3490,7 @@
         <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D64" t="s">
         <v>56</v>
@@ -3530,7 +3530,7 @@
         <v>56</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D65" t="s">
         <v>56</v>
@@ -3570,7 +3570,7 @@
         <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D66" t="s">
         <v>56</v>
@@ -3608,7 +3608,7 @@
         <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D67" t="s">
         <v>56</v>
@@ -3646,7 +3646,7 @@
         <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D68" t="s">
         <v>56</v>
@@ -3688,7 +3688,7 @@
         <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D69" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
check maven parameters in jenkins
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46878E01-9D4F-4D99-BA7F-71C4AAA54830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C79AE09-ECFF-4351-B32D-2E801C6A6329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E95F9A-57EF-44F9-A697-55E309233EEF}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +867,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -900,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38982D-3F95-4179-9809-2B80AF189016}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add jenkins build details as parameterize
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E1A044-01E4-4C5D-B7F7-6E0ED79A82A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9B8996-6763-4B79-B0E7-236EBE306051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38982D-3F95-4179-9809-2B80AF189016}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,7 +986,7 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1258,7 +1258,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
@@ -1300,7 +1300,7 @@
         <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
         <v>56</v>
@@ -1340,7 +1340,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>56</v>
@@ -1380,7 +1380,7 @@
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>56</v>
@@ -1420,7 +1420,7 @@
         <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>56</v>
@@ -1500,7 +1500,7 @@
         <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>56</v>
@@ -1540,7 +1540,7 @@
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
@@ -1580,7 +1580,7 @@
         <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>56</v>
@@ -1620,7 +1620,7 @@
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -1660,7 +1660,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
@@ -1698,7 +1698,7 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
@@ -1736,7 +1736,7 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
@@ -1778,7 +1778,7 @@
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
@@ -1896,7 +1896,7 @@
         <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
         <v>56</v>
@@ -1938,7 +1938,7 @@
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
         <v>56</v>
@@ -1978,7 +1978,7 @@
         <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
         <v>56</v>
@@ -2018,7 +2018,7 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
         <v>56</v>
@@ -2058,7 +2058,7 @@
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
         <v>56</v>
@@ -2098,7 +2098,7 @@
         <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -2138,7 +2138,7 @@
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
         <v>56</v>
@@ -2178,7 +2178,7 @@
         <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
         <v>56</v>
@@ -2218,7 +2218,7 @@
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
         <v>56</v>
@@ -2258,7 +2258,7 @@
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -2298,7 +2298,7 @@
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
         <v>56</v>
@@ -2336,7 +2336,7 @@
         <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
         <v>56</v>
@@ -2374,7 +2374,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
         <v>56</v>
@@ -2416,7 +2416,7 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
         <v>56</v>
@@ -2534,7 +2534,7 @@
         <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
         <v>56</v>
@@ -2576,7 +2576,7 @@
         <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
         <v>56</v>
@@ -2616,7 +2616,7 @@
         <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s">
         <v>56</v>
@@ -2656,7 +2656,7 @@
         <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s">
         <v>56</v>
@@ -2696,7 +2696,7 @@
         <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s">
         <v>56</v>
@@ -2736,7 +2736,7 @@
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
         <v>56</v>
@@ -2776,7 +2776,7 @@
         <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
         <v>56</v>
@@ -2816,7 +2816,7 @@
         <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
         <v>56</v>
@@ -2856,7 +2856,7 @@
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s">
         <v>56</v>
@@ -2896,7 +2896,7 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
         <v>56</v>
@@ -2936,7 +2936,7 @@
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
         <v>56</v>
@@ -2974,7 +2974,7 @@
         <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s">
         <v>56</v>
@@ -3012,7 +3012,7 @@
         <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D52" t="s">
         <v>56</v>
@@ -3054,7 +3054,7 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D53" t="s">
         <v>56</v>
@@ -3172,7 +3172,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s">
         <v>56</v>
@@ -3214,7 +3214,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
         <v>56</v>
@@ -3254,7 +3254,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
         <v>56</v>
@@ -3294,7 +3294,7 @@
         <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D59" t="s">
         <v>56</v>
@@ -3334,7 +3334,7 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
         <v>56</v>
@@ -3374,7 +3374,7 @@
         <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D61" t="s">
         <v>56</v>
@@ -3414,7 +3414,7 @@
         <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D62" t="s">
         <v>56</v>
@@ -3454,7 +3454,7 @@
         <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
         <v>56</v>
@@ -3494,7 +3494,7 @@
         <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D64" t="s">
         <v>56</v>
@@ -3534,7 +3534,7 @@
         <v>56</v>
       </c>
       <c r="C65" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s">
         <v>56</v>
@@ -3574,7 +3574,7 @@
         <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D66" t="s">
         <v>56</v>
@@ -3612,7 +3612,7 @@
         <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D67" t="s">
         <v>56</v>
@@ -3650,7 +3650,7 @@
         <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s">
         <v>56</v>
@@ -3692,7 +3692,7 @@
         <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
check Login in Jenkins
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6E5B1F-265F-413A-857E-081BBFE031C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130C9C35-8F07-4FCC-B98F-770D54BE1C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -431,9 +431,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>VD84ekKYun@gmail.com</t>
-  </si>
-  <si>
     <t>sdjgsoghur@gmail.com</t>
   </si>
   <si>
@@ -453,6 +450,9 @@
   </si>
   <si>
     <t>Password should contain at least one non-alphanumeric character</t>
+  </si>
+  <si>
+    <t>jqetgFWHup@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -835,7 +835,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +870,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -884,7 +884,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38982D-3F95-4179-9809-2B80AF189016}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,7 +986,7 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1043,7 +1043,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
@@ -1089,7 +1089,7 @@
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>56</v>
@@ -1135,7 +1135,7 @@
         <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>56</v>
@@ -1258,7 +1258,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
@@ -1529,7 +1529,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -2167,7 +2167,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
@@ -2805,7 +2805,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
@@ -3443,7 +3443,7 @@
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.3">
@@ -3767,8 +3767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D389FA8-13DD-4536-81A5-8107290E082A}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3812,7 +3812,7 @@
         <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
@@ -3832,7 +3832,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -3840,7 +3840,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
@@ -3857,7 +3857,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
@@ -3889,7 +3889,7 @@
         <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3899,8 +3899,8 @@
     <hyperlink ref="F3" r:id="rId3" xr:uid="{A7CA78D2-A9CB-48A9-B3A2-2856EC5418F2}"/>
     <hyperlink ref="E3" r:id="rId4" xr:uid="{4F77765E-F229-4668-8B1F-BB91864EDB8A}"/>
     <hyperlink ref="F4" r:id="rId5" xr:uid="{9EC47F56-16A1-4DAC-B49C-35B8730D81AD}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{3F257CFF-DC38-4B3E-A7AE-B78523B06DCF}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{B9C65906-6D48-43F8-BB4E-93B75382193E}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{B904A858-406E-4F64-8853-8A94CE624CC2}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{FC67305E-CBAC-4104-A0BA-832C9DDEC1B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
my account scenarios added check captcha verification
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14A5055-57A2-4E42-99D6-D23CF82F4E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AF1A85-28FE-41C3-BA73-538D70FEB3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
     <sheet name="Registration" sheetId="1" r:id="rId2"/>
     <sheet name="Login" sheetId="2" r:id="rId3"/>
+    <sheet name="MyAccount" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Registration!$A$1:$T$69</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="165">
   <si>
     <t>TestName</t>
   </si>
@@ -456,6 +457,75 @@
   </si>
   <si>
     <t>U2ux5ANnR9@gmail.com</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>MyAccount</t>
+  </si>
+  <si>
+    <t>Expected_Error</t>
+  </si>
+  <si>
+    <t>Old password and new password should not be same</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_samenegativeflow_1</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_negativeflow_1</t>
+  </si>
+  <si>
+    <t>asdfadsfas</t>
+  </si>
+  <si>
+    <t>At least one upper case char</t>
+  </si>
+  <si>
+    <t>At least one lower case char</t>
+  </si>
+  <si>
+    <t>23443212</t>
+  </si>
+  <si>
+    <t>Nsdgs234</t>
+  </si>
+  <si>
+    <t>At least one non alpha numeric char (@,!,#, etc)</t>
+  </si>
+  <si>
+    <t>Jsdfsdg@</t>
+  </si>
+  <si>
+    <t>At least one number digit</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_negativeflow_2</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_negativeflow_3</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_negativeflow_4</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_negativeflow_5</t>
+  </si>
+  <si>
+    <t>Should be at least 8 chars</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>Sgidfe345@</t>
+  </si>
+  <si>
+    <t>TC_appchangepassword_erroroldpasswordflow_1</t>
+  </si>
+  <si>
+    <t>Incorrect old password, please try again with the correct password</t>
   </si>
 </sst>
 </file>
@@ -835,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E95F9A-57EF-44F9-A697-55E309233EEF}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,7 +943,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -887,9 +957,23 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3770,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D389FA8-13DD-4536-81A5-8107290E082A}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3908,4 +3992,253 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F22930-2B4B-4ECB-95E3-2CA3D85E1A3B}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{295AE882-2DF8-4C52-BCC5-272AF1488C33}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{FBDF0631-83E1-4D2E-9F48-B40235C48FD0}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{C70C7F0E-DA9D-43DD-8585-A8D797B68999}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{8099DEDE-C1F6-482C-949B-26CD83F5AA5C}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{793C0D70-8E75-4D00-A69E-9699326AEE9C}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{3785A2FF-4DEE-4C1A-BF12-4A3790864C66}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{3D3062FC-D8C4-468A-89F4-BAACDE63FF09}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{3903EEE1-32E0-4C87-9FFC-0FFC629210D6}"/>
+    <hyperlink ref="F4" r:id="rId9" xr:uid="{32419C80-3F50-42DF-B337-2AC8C6F987AC}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{8A21FEDB-B7FF-4A57-B902-E3E084BDE91F}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{B6CB6B95-0774-4538-9072-07F46A5B7505}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{ADF0FAE6-EB7A-4C20-BF57-BCD6EAA59F50}"/>
+    <hyperlink ref="F7" r:id="rId13" xr:uid="{E92B2622-A663-4F49-A033-F6EC6C8CC631}"/>
+    <hyperlink ref="E8" r:id="rId14" xr:uid="{5B5B3BE6-CAF4-429B-9934-7D143B88453F}"/>
+    <hyperlink ref="F8" r:id="rId15" xr:uid="{0F6B3EC9-51AA-49E0-9A9D-94FEBD8AF56E}"/>
+    <hyperlink ref="G8" r:id="rId16" xr:uid="{7F6287CC-BB92-4E52-809C-EB767EC74917}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
enter text component updated
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C66AEF-EDC0-4D3D-87FE-8BC772F35DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7BF462-137F-41CF-BA1A-DB5A11B928B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1036,7 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -1050,7 +1050,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
dynamic wait logic is updated
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7BF462-137F-41CF-BA1A-DB5A11B928B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC14929-10F6-4CD5-B2BA-6D72A89BD53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E95F9A-57EF-44F9-A697-55E309233EEF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38982D-3F95-4179-9809-2B80AF189016}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1358,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -1398,7 +1398,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -1438,7 +1438,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -1480,7 +1480,7 @@
         <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
@@ -1520,7 +1520,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>54</v>
@@ -1560,7 +1560,7 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
@@ -1600,7 +1600,7 @@
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>54</v>
@@ -1640,7 +1640,7 @@
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
@@ -1680,7 +1680,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>54</v>
@@ -1720,7 +1720,7 @@
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
@@ -1760,7 +1760,7 @@
         <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
         <v>54</v>
@@ -1800,7 +1800,7 @@
         <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>54</v>
@@ -1840,7 +1840,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
@@ -1878,7 +1878,7 @@
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
@@ -1916,7 +1916,7 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
@@ -1958,7 +1958,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
         <v>54</v>
@@ -1996,7 +1996,7 @@
         <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
@@ -2036,7 +2036,7 @@
         <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
         <v>54</v>
@@ -2076,7 +2076,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
         <v>54</v>
@@ -2118,7 +2118,7 @@
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
         <v>54</v>
@@ -2158,7 +2158,7 @@
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
         <v>54</v>
@@ -2198,7 +2198,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -2238,7 +2238,7 @@
         <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
         <v>54</v>
@@ -2278,7 +2278,7 @@
         <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
@@ -2318,7 +2318,7 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
         <v>54</v>
@@ -2358,7 +2358,7 @@
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
         <v>54</v>
@@ -2398,7 +2398,7 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
         <v>54</v>
@@ -2438,7 +2438,7 @@
         <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
         <v>54</v>
@@ -2478,7 +2478,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
         <v>54</v>
@@ -2516,7 +2516,7 @@
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
         <v>54</v>
@@ -2554,7 +2554,7 @@
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
         <v>54</v>
@@ -2596,7 +2596,7 @@
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
         <v>54</v>
@@ -2634,7 +2634,7 @@
         <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
         <v>54</v>
@@ -2674,7 +2674,7 @@
         <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D39" t="s">
         <v>54</v>
@@ -2714,7 +2714,7 @@
         <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D40" t="s">
         <v>54</v>
@@ -2756,7 +2756,7 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
         <v>54</v>
@@ -2796,7 +2796,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D42" t="s">
         <v>54</v>
@@ -2836,7 +2836,7 @@
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -2876,7 +2876,7 @@
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
         <v>54</v>
@@ -2916,7 +2916,7 @@
         <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D45" t="s">
         <v>54</v>
@@ -2956,7 +2956,7 @@
         <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D46" t="s">
         <v>54</v>
@@ -2996,7 +2996,7 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D47" t="s">
         <v>54</v>
@@ -3036,7 +3036,7 @@
         <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
         <v>54</v>
@@ -3076,7 +3076,7 @@
         <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D49" t="s">
         <v>54</v>
@@ -3116,7 +3116,7 @@
         <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D50" t="s">
         <v>54</v>
@@ -3154,7 +3154,7 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D51" t="s">
         <v>54</v>
@@ -3192,7 +3192,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -3234,7 +3234,7 @@
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D53" t="s">
         <v>54</v>
@@ -3272,7 +3272,7 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D54" t="s">
         <v>54</v>
@@ -3312,7 +3312,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D55" t="s">
         <v>54</v>
@@ -3352,7 +3352,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D56" t="s">
         <v>54</v>
@@ -3394,7 +3394,7 @@
         <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D57" t="s">
         <v>54</v>
@@ -3434,7 +3434,7 @@
         <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D58" t="s">
         <v>54</v>
@@ -3474,7 +3474,7 @@
         <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D59" t="s">
         <v>54</v>
@@ -3514,7 +3514,7 @@
         <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D60" t="s">
         <v>54</v>
@@ -3554,7 +3554,7 @@
         <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
         <v>54</v>
@@ -3594,7 +3594,7 @@
         <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D62" t="s">
         <v>54</v>
@@ -3634,7 +3634,7 @@
         <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D63" t="s">
         <v>54</v>
@@ -3674,7 +3674,7 @@
         <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D64" t="s">
         <v>54</v>
@@ -3714,7 +3714,7 @@
         <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D65" t="s">
         <v>54</v>
@@ -3754,7 +3754,7 @@
         <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D66" t="s">
         <v>54</v>
@@ -3792,7 +3792,7 @@
         <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D67" t="s">
         <v>54</v>
@@ -3830,7 +3830,7 @@
         <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D68" t="s">
         <v>54</v>
@@ -3872,7 +3872,7 @@
         <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D69" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
profile setting test cases added
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C12CE5-B66C-4875-8430-274DF88DCEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F19E4D6-1BAE-43E8-868B-739B7871DA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{460863B9-487A-435D-AEBE-1644A7825E30}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="255">
   <si>
     <t>TestName</t>
   </si>
@@ -619,6 +619,183 @@
   </si>
   <si>
     <t>Ef0aNn38tp@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_1</t>
+  </si>
+  <si>
+    <t>TestAdd1</t>
+  </si>
+  <si>
+    <t>TestAdd2</t>
+  </si>
+  <si>
+    <t>chicago</t>
+  </si>
+  <si>
+    <t>60005</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_2</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_3</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_4</t>
+  </si>
+  <si>
+    <t>TestAutoFN849</t>
+  </si>
+  <si>
+    <t>TestAutoLN9494</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_5</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_6</t>
+  </si>
+  <si>
+    <t>iujhikjdfowerfoihdgfoihj</t>
+  </si>
+  <si>
+    <t>Name can contain only alphabets</t>
+  </si>
+  <si>
+    <t>First Name has to be less than or equal to 20 characters.</t>
+  </si>
+  <si>
+    <t>Last Name has to be less than or equal to 20 characters.</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_1</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_2</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_3</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_4</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_5</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_6</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_1</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_2</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_3</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_4</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_5</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_6</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_1</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_2</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_3</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_4</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_5</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_6</t>
+  </si>
+  <si>
+    <t>EcEtRWLQea@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_7</t>
+  </si>
+  <si>
+    <t>9458</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_8</t>
+  </si>
+  <si>
+    <t>D/M/YYYY</t>
+  </si>
+  <si>
+    <t>Phone number is not valid</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_9</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_MusicSchool_10</t>
+  </si>
+  <si>
+    <t>First Name is required!</t>
+  </si>
+  <si>
+    <t>Last Name is required!</t>
+  </si>
+  <si>
+    <t>TC_myprofile_DOBnegativeflow_MusicSchool_11</t>
+  </si>
+  <si>
+    <t>DOB should not be current date</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_7</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_8</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_9</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Parent_10</t>
+  </si>
+  <si>
+    <t>TC_myprofile_DOBnegativeflow_Parent_11</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_7</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_8</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_9</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Teacher_10</t>
+  </si>
+  <si>
+    <t>TC_myprofile_DOBnegativeflow_Teacher_11</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1178,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1213,7 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -1050,7 +1227,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -1080,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38982D-3F95-4179-9809-2B80AF189016}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1343,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -1223,7 +1400,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -1315,7 +1492,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -1438,7 +1615,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -1480,7 +1657,7 @@
         <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
@@ -1520,7 +1697,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>54</v>
@@ -1560,7 +1737,7 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
@@ -1600,7 +1777,7 @@
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>54</v>
@@ -1640,7 +1817,7 @@
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
@@ -1680,7 +1857,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>54</v>
@@ -1720,7 +1897,7 @@
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
@@ -1760,7 +1937,7 @@
         <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
         <v>54</v>
@@ -1800,7 +1977,7 @@
         <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>54</v>
@@ -1840,7 +2017,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
@@ -1878,7 +2055,7 @@
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
@@ -1916,7 +2093,7 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
@@ -1958,7 +2135,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>54</v>
@@ -2076,7 +2253,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
         <v>54</v>
@@ -2118,7 +2295,7 @@
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
         <v>54</v>
@@ -2158,7 +2335,7 @@
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>54</v>
@@ -2198,7 +2375,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -2238,7 +2415,7 @@
         <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
         <v>54</v>
@@ -2278,7 +2455,7 @@
         <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
@@ -2318,7 +2495,7 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>54</v>
@@ -2358,7 +2535,7 @@
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
         <v>54</v>
@@ -2398,7 +2575,7 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
         <v>54</v>
@@ -2438,7 +2615,7 @@
         <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>54</v>
@@ -2478,7 +2655,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
         <v>54</v>
@@ -2516,7 +2693,7 @@
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
         <v>54</v>
@@ -2554,7 +2731,7 @@
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
         <v>54</v>
@@ -2596,7 +2773,7 @@
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
         <v>54</v>
@@ -2714,7 +2891,7 @@
         <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
         <v>54</v>
@@ -2756,7 +2933,7 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
         <v>54</v>
@@ -2796,7 +2973,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
         <v>54</v>
@@ -2836,7 +3013,7 @@
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -2876,7 +3053,7 @@
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
         <v>54</v>
@@ -2916,7 +3093,7 @@
         <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
         <v>54</v>
@@ -2956,7 +3133,7 @@
         <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
         <v>54</v>
@@ -2996,7 +3173,7 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D47" t="s">
         <v>54</v>
@@ -3036,7 +3213,7 @@
         <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D48" t="s">
         <v>54</v>
@@ -3076,7 +3253,7 @@
         <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
         <v>54</v>
@@ -3116,7 +3293,7 @@
         <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
         <v>54</v>
@@ -3154,7 +3331,7 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
         <v>54</v>
@@ -3192,7 +3369,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -3234,7 +3411,7 @@
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D53" t="s">
         <v>54</v>
@@ -3352,7 +3529,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D56" t="s">
         <v>54</v>
@@ -3394,7 +3571,7 @@
         <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D57" t="s">
         <v>54</v>
@@ -3434,7 +3611,7 @@
         <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D58" t="s">
         <v>54</v>
@@ -3474,7 +3651,7 @@
         <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D59" t="s">
         <v>54</v>
@@ -3514,7 +3691,7 @@
         <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
         <v>54</v>
@@ -3554,7 +3731,7 @@
         <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D61" t="s">
         <v>54</v>
@@ -3594,7 +3771,7 @@
         <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D62" t="s">
         <v>54</v>
@@ -3634,7 +3811,7 @@
         <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D63" t="s">
         <v>54</v>
@@ -3674,7 +3851,7 @@
         <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D64" t="s">
         <v>54</v>
@@ -3714,7 +3891,7 @@
         <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D65" t="s">
         <v>54</v>
@@ -3754,7 +3931,7 @@
         <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s">
         <v>54</v>
@@ -3792,7 +3969,7 @@
         <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D67" t="s">
         <v>54</v>
@@ -3830,7 +4007,7 @@
         <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D68" t="s">
         <v>54</v>
@@ -3872,7 +4049,7 @@
         <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D69" t="s">
         <v>54</v>
@@ -4089,10 +4266,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F22930-2B4B-4ECB-95E3-2CA3D85E1A3B}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4103,9 +4280,13 @@
     <col min="6" max="6" width="20.109375" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.5546875" customWidth="1"/>
+    <col min="9" max="10" width="19.21875" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4130,10 +4311,43 @@
       <c r="H1" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -4145,19 +4359,52 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>197</v>
+      </c>
+      <c r="O2" t="s">
+        <v>198</v>
+      </c>
+      <c r="P2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" t="s">
+        <v>201</v>
+      </c>
+      <c r="S2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -4169,21 +4416,52 @@
         <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>144</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>197</v>
+      </c>
+      <c r="O3" t="s">
+        <v>198</v>
+      </c>
+      <c r="P3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R3" t="s">
+        <v>201</v>
+      </c>
+      <c r="S3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -4195,21 +4473,52 @@
         <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J4" t="s">
+        <v>157</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>197</v>
+      </c>
+      <c r="O4" t="s">
+        <v>198</v>
+      </c>
+      <c r="P4" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R4" t="s">
+        <v>201</v>
+      </c>
+      <c r="S4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
@@ -4221,21 +4530,52 @@
         <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
-        <v>148</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J5" t="s">
+        <v>208</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>197</v>
+      </c>
+      <c r="O5" t="s">
+        <v>198</v>
+      </c>
+      <c r="P5" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R5" t="s">
+        <v>201</v>
+      </c>
+      <c r="S5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -4247,21 +4587,52 @@
         <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+      <c r="I6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" t="s">
+        <v>197</v>
+      </c>
+      <c r="O6" t="s">
+        <v>198</v>
+      </c>
+      <c r="P6" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R6" t="s">
+        <v>201</v>
+      </c>
+      <c r="S6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -4273,21 +4644,52 @@
         <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>153</v>
-      </c>
+      <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="I7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J7" t="s">
+        <v>211</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" t="s">
+        <v>197</v>
+      </c>
+      <c r="O7" t="s">
+        <v>198</v>
+      </c>
+      <c r="P7" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R7" t="s">
+        <v>201</v>
+      </c>
+      <c r="S7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -4299,21 +4701,52 @@
         <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+      <c r="I8" t="s">
+        <v>156</v>
+      </c>
+      <c r="J8" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
+        <v>197</v>
+      </c>
+      <c r="O8" t="s">
+        <v>198</v>
+      </c>
+      <c r="P8" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R8" t="s">
+        <v>201</v>
+      </c>
+      <c r="S8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>236</v>
       </c>
       <c r="B9" t="s">
         <v>54</v>
@@ -4325,19 +4758,52 @@
         <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>194</v>
+        <v>139</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="I9" t="s">
+        <v>156</v>
+      </c>
+      <c r="J9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N9" t="s">
+        <v>197</v>
+      </c>
+      <c r="O9" t="s">
+        <v>198</v>
+      </c>
+      <c r="P9" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R9" t="s">
+        <v>201</v>
+      </c>
+      <c r="S9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>239</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
@@ -4349,21 +4815,50 @@
         <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>194</v>
+        <v>139</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G10" t="s">
-        <v>144</v>
-      </c>
+      <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>197</v>
+      </c>
+      <c r="O10" t="s">
+        <v>198</v>
+      </c>
+      <c r="P10" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R10" t="s">
+        <v>201</v>
+      </c>
+      <c r="S10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
@@ -4375,21 +4870,50 @@
         <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>194</v>
+        <v>139</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="I11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" t="s">
+        <v>197</v>
+      </c>
+      <c r="O11" t="s">
+        <v>198</v>
+      </c>
+      <c r="P11" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R11" t="s">
+        <v>201</v>
+      </c>
+      <c r="S11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>243</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -4401,21 +4925,52 @@
         <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>194</v>
+        <v>139</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G12" t="s">
-        <v>148</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="I12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J12" t="s">
+        <v>157</v>
+      </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" t="s">
+        <v>197</v>
+      </c>
+      <c r="O12" t="s">
+        <v>198</v>
+      </c>
+      <c r="P12" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R12" t="s">
+        <v>201</v>
+      </c>
+      <c r="S12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
@@ -4427,21 +4982,52 @@
         <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" t="s">
+        <v>197</v>
+      </c>
+      <c r="O13" t="s">
+        <v>198</v>
+      </c>
+      <c r="P13" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R13" t="s">
+        <v>201</v>
+      </c>
+      <c r="S13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
@@ -4453,21 +5039,52 @@
         <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G14" t="s">
-        <v>153</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I14" t="s">
+        <v>156</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" t="s">
+        <v>197</v>
+      </c>
+      <c r="O14" t="s">
+        <v>198</v>
+      </c>
+      <c r="P14" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R14" t="s">
+        <v>201</v>
+      </c>
+      <c r="S14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
@@ -4479,21 +5096,52 @@
         <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I15" t="s">
+        <v>207</v>
+      </c>
+      <c r="J15" t="s">
+        <v>157</v>
+      </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>197</v>
+      </c>
+      <c r="O15" t="s">
+        <v>198</v>
+      </c>
+      <c r="P15" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R15" t="s">
+        <v>201</v>
+      </c>
+      <c r="S15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
@@ -4505,19 +5153,52 @@
         <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I16" t="s">
+        <v>156</v>
+      </c>
+      <c r="J16" t="s">
+        <v>208</v>
+      </c>
+      <c r="K16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" t="s">
+        <v>197</v>
+      </c>
+      <c r="O16" t="s">
+        <v>198</v>
+      </c>
+      <c r="P16" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R16" t="s">
+        <v>201</v>
+      </c>
+      <c r="S16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
@@ -4529,21 +5210,52 @@
         <v>54</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G17" t="s">
-        <v>144</v>
-      </c>
+      <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+      <c r="I17" t="s">
+        <v>211</v>
+      </c>
+      <c r="J17" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N17" t="s">
+        <v>197</v>
+      </c>
+      <c r="O17" t="s">
+        <v>198</v>
+      </c>
+      <c r="P17" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R17" t="s">
+        <v>201</v>
+      </c>
+      <c r="S17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
@@ -4555,21 +5267,52 @@
         <v>54</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="I18" t="s">
+        <v>156</v>
+      </c>
+      <c r="J18" t="s">
+        <v>211</v>
+      </c>
+      <c r="K18" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" t="s">
+        <v>197</v>
+      </c>
+      <c r="O18" t="s">
+        <v>198</v>
+      </c>
+      <c r="P18" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R18" t="s">
+        <v>201</v>
+      </c>
+      <c r="S18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
@@ -4581,21 +5324,52 @@
         <v>54</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G19" t="s">
-        <v>148</v>
-      </c>
+      <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+      <c r="I19" t="s">
+        <v>156</v>
+      </c>
+      <c r="J19" t="s">
+        <v>157</v>
+      </c>
+      <c r="K19" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19" t="s">
+        <v>197</v>
+      </c>
+      <c r="O19" t="s">
+        <v>198</v>
+      </c>
+      <c r="P19" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R19" t="s">
+        <v>201</v>
+      </c>
+      <c r="S19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>246</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
@@ -4607,21 +5381,52 @@
         <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="I20" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" t="s">
+        <v>157</v>
+      </c>
+      <c r="K20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N20" t="s">
+        <v>197</v>
+      </c>
+      <c r="O20" t="s">
+        <v>198</v>
+      </c>
+      <c r="P20" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R20" t="s">
+        <v>201</v>
+      </c>
+      <c r="S20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>247</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
@@ -4633,21 +5438,50 @@
         <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G21" t="s">
-        <v>153</v>
-      </c>
+      <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" t="s">
+        <v>157</v>
+      </c>
+      <c r="K21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" t="s">
+        <v>197</v>
+      </c>
+      <c r="O21" t="s">
+        <v>198</v>
+      </c>
+      <c r="P21" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R21" t="s">
+        <v>201</v>
+      </c>
+      <c r="S21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>248</v>
       </c>
       <c r="B22" t="s">
         <v>54</v>
@@ -4659,21 +5493,50 @@
         <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="I22" t="s">
+        <v>156</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" t="s">
+        <v>197</v>
+      </c>
+      <c r="O22" t="s">
+        <v>198</v>
+      </c>
+      <c r="P22" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R22" t="s">
+        <v>201</v>
+      </c>
+      <c r="S22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
@@ -4685,19 +5548,52 @@
         <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="I23" t="s">
+        <v>156</v>
+      </c>
+      <c r="J23" t="s">
+        <v>157</v>
+      </c>
+      <c r="K23" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" t="s">
+        <v>197</v>
+      </c>
+      <c r="O23" t="s">
+        <v>198</v>
+      </c>
+      <c r="P23" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R23" t="s">
+        <v>201</v>
+      </c>
+      <c r="S23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -4709,21 +5605,52 @@
         <v>54</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G24" t="s">
-        <v>144</v>
-      </c>
+      <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" t="s">
+        <v>157</v>
+      </c>
+      <c r="K24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" t="s">
+        <v>197</v>
+      </c>
+      <c r="O24" t="s">
+        <v>198</v>
+      </c>
+      <c r="P24" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R24" t="s">
+        <v>201</v>
+      </c>
+      <c r="S24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>222</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -4735,21 +5662,52 @@
         <v>54</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I25" t="s">
+        <v>156</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" t="s">
+        <v>197</v>
+      </c>
+      <c r="O25" t="s">
+        <v>198</v>
+      </c>
+      <c r="P25" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R25" t="s">
+        <v>201</v>
+      </c>
+      <c r="S25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
@@ -4761,21 +5719,52 @@
         <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G26" t="s">
-        <v>148</v>
-      </c>
+      <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I26" t="s">
+        <v>207</v>
+      </c>
+      <c r="J26" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" t="s">
+        <v>197</v>
+      </c>
+      <c r="O26" t="s">
+        <v>198</v>
+      </c>
+      <c r="P26" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R26" t="s">
+        <v>201</v>
+      </c>
+      <c r="S26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="B27" t="s">
         <v>54</v>
@@ -4787,21 +5776,52 @@
         <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="I27" t="s">
+        <v>156</v>
+      </c>
+      <c r="J27" t="s">
+        <v>208</v>
+      </c>
+      <c r="K27" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27" t="s">
+        <v>197</v>
+      </c>
+      <c r="O27" t="s">
+        <v>198</v>
+      </c>
+      <c r="P27" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R27" t="s">
+        <v>201</v>
+      </c>
+      <c r="S27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
@@ -4813,21 +5833,52 @@
         <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G28" t="s">
-        <v>153</v>
-      </c>
+      <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+      <c r="I28" t="s">
+        <v>211</v>
+      </c>
+      <c r="J28" t="s">
+        <v>157</v>
+      </c>
+      <c r="K28" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" t="s">
+        <v>197</v>
+      </c>
+      <c r="O28" t="s">
+        <v>198</v>
+      </c>
+      <c r="P28" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R28" t="s">
+        <v>201</v>
+      </c>
+      <c r="S28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -4839,77 +5890,1512 @@
         <v>54</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="I29" t="s">
+        <v>156</v>
+      </c>
+      <c r="J29" t="s">
+        <v>211</v>
+      </c>
+      <c r="K29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" t="s">
+        <v>197</v>
+      </c>
+      <c r="O29" t="s">
+        <v>198</v>
+      </c>
+      <c r="P29" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R29" t="s">
+        <v>201</v>
+      </c>
+      <c r="S29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>250</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>139</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" t="s">
+        <v>238</v>
+      </c>
+      <c r="I30" t="s">
+        <v>156</v>
+      </c>
+      <c r="J30" t="s">
+        <v>157</v>
+      </c>
+      <c r="K30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N30" t="s">
+        <v>197</v>
+      </c>
+      <c r="O30" t="s">
+        <v>198</v>
+      </c>
+      <c r="P30" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R30" t="s">
+        <v>201</v>
+      </c>
+      <c r="S30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" t="s">
+        <v>214</v>
+      </c>
+      <c r="I31" t="s">
+        <v>156</v>
+      </c>
+      <c r="J31" t="s">
+        <v>157</v>
+      </c>
+      <c r="K31" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N31" t="s">
+        <v>197</v>
+      </c>
+      <c r="O31" t="s">
+        <v>198</v>
+      </c>
+      <c r="P31" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R31" t="s">
+        <v>201</v>
+      </c>
+      <c r="S31" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" t="s">
+        <v>241</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" t="s">
+        <v>157</v>
+      </c>
+      <c r="K32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32" t="s">
+        <v>197</v>
+      </c>
+      <c r="O32" t="s">
+        <v>198</v>
+      </c>
+      <c r="P32" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R32" t="s">
+        <v>201</v>
+      </c>
+      <c r="S32" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" t="s">
+        <v>242</v>
+      </c>
+      <c r="I33" t="s">
+        <v>156</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" t="s">
+        <v>197</v>
+      </c>
+      <c r="O33" t="s">
+        <v>198</v>
+      </c>
+      <c r="P33" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R33" t="s">
+        <v>201</v>
+      </c>
+      <c r="S33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>254</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" t="s">
+        <v>244</v>
+      </c>
+      <c r="I34" t="s">
+        <v>156</v>
+      </c>
+      <c r="J34" t="s">
+        <v>157</v>
+      </c>
+      <c r="K34" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" t="s">
+        <v>197</v>
+      </c>
+      <c r="O34" t="s">
+        <v>198</v>
+      </c>
+      <c r="P34" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R34" t="s">
+        <v>201</v>
+      </c>
+      <c r="S34" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>227</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" t="s">
+        <v>212</v>
+      </c>
+      <c r="I35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" t="s">
+        <v>157</v>
+      </c>
+      <c r="K35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" t="s">
+        <v>197</v>
+      </c>
+      <c r="O35" t="s">
+        <v>198</v>
+      </c>
+      <c r="P35" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R35" t="s">
+        <v>201</v>
+      </c>
+      <c r="S35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" t="s">
+        <v>212</v>
+      </c>
+      <c r="I36" t="s">
+        <v>156</v>
+      </c>
+      <c r="J36" t="s">
+        <v>30</v>
+      </c>
+      <c r="K36" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" t="s">
+        <v>197</v>
+      </c>
+      <c r="O36" t="s">
+        <v>198</v>
+      </c>
+      <c r="P36" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R36" t="s">
+        <v>201</v>
+      </c>
+      <c r="S36" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>229</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" t="s">
+        <v>212</v>
+      </c>
+      <c r="I37" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" t="s">
+        <v>157</v>
+      </c>
+      <c r="K37" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" t="s">
+        <v>197</v>
+      </c>
+      <c r="O37" t="s">
+        <v>198</v>
+      </c>
+      <c r="P37" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R37" t="s">
+        <v>201</v>
+      </c>
+      <c r="S37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" t="s">
+        <v>212</v>
+      </c>
+      <c r="I38" t="s">
+        <v>156</v>
+      </c>
+      <c r="J38" t="s">
+        <v>208</v>
+      </c>
+      <c r="K38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" t="s">
+        <v>197</v>
+      </c>
+      <c r="O38" t="s">
+        <v>198</v>
+      </c>
+      <c r="P38" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R38" t="s">
+        <v>201</v>
+      </c>
+      <c r="S38" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" t="s">
+        <v>213</v>
+      </c>
+      <c r="I39" t="s">
+        <v>211</v>
+      </c>
+      <c r="J39" t="s">
+        <v>157</v>
+      </c>
+      <c r="K39" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N39" t="s">
+        <v>197</v>
+      </c>
+      <c r="O39" t="s">
+        <v>198</v>
+      </c>
+      <c r="P39" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R39" t="s">
+        <v>201</v>
+      </c>
+      <c r="S39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" t="s">
+        <v>214</v>
+      </c>
+      <c r="I40" t="s">
+        <v>156</v>
+      </c>
+      <c r="J40" t="s">
+        <v>211</v>
+      </c>
+      <c r="K40" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N40" t="s">
+        <v>197</v>
+      </c>
+      <c r="O40" t="s">
+        <v>198</v>
+      </c>
+      <c r="P40" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R40" t="s">
+        <v>201</v>
+      </c>
+      <c r="S40" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s">
+        <v>144</v>
+      </c>
+      <c r="H42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" t="s">
+        <v>148</v>
+      </c>
+      <c r="H44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" t="s">
+        <v>144</v>
+      </c>
+      <c r="H49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" t="s">
+        <v>148</v>
+      </c>
+      <c r="H51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" t="s">
+        <v>153</v>
+      </c>
+      <c r="H53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" t="s">
+        <v>54</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" t="s">
+        <v>144</v>
+      </c>
+      <c r="H56" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" t="s">
+        <v>54</v>
+      </c>
+      <c r="D58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" t="s">
+        <v>148</v>
+      </c>
+      <c r="H58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" t="s">
+        <v>54</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" t="s">
+        <v>144</v>
+      </c>
+      <c r="H63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" t="s">
+        <v>54</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>190</v>
+      </c>
+      <c r="B65" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" t="s">
+        <v>148</v>
+      </c>
+      <c r="H65" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" t="s">
+        <v>54</v>
+      </c>
+      <c r="D66" t="s">
+        <v>54</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H66" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" t="s">
+        <v>54</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G67" t="s">
+        <v>153</v>
+      </c>
+      <c r="H67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H68" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{295AE882-2DF8-4C52-BCC5-272AF1488C33}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{FBDF0631-83E1-4D2E-9F48-B40235C48FD0}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{C70C7F0E-DA9D-43DD-8585-A8D797B68999}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{8099DEDE-C1F6-482C-949B-26CD83F5AA5C}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{793C0D70-8E75-4D00-A69E-9699326AEE9C}"/>
-    <hyperlink ref="E4" r:id="rId6" xr:uid="{3785A2FF-4DEE-4C1A-BF12-4A3790864C66}"/>
-    <hyperlink ref="E5" r:id="rId7" xr:uid="{3D3062FC-D8C4-468A-89F4-BAACDE63FF09}"/>
-    <hyperlink ref="E6" r:id="rId8" xr:uid="{3903EEE1-32E0-4C87-9FFC-0FFC629210D6}"/>
-    <hyperlink ref="F4" r:id="rId9" xr:uid="{32419C80-3F50-42DF-B337-2AC8C6F987AC}"/>
-    <hyperlink ref="F5" r:id="rId10" xr:uid="{8A21FEDB-B7FF-4A57-B902-E3E084BDE91F}"/>
-    <hyperlink ref="F6" r:id="rId11" xr:uid="{B6CB6B95-0774-4538-9072-07F46A5B7505}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{ADF0FAE6-EB7A-4C20-BF57-BCD6EAA59F50}"/>
-    <hyperlink ref="F7" r:id="rId13" xr:uid="{E92B2622-A663-4F49-A033-F6EC6C8CC631}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{5B5B3BE6-CAF4-429B-9934-7D143B88453F}"/>
-    <hyperlink ref="F8" r:id="rId15" xr:uid="{0F6B3EC9-51AA-49E0-9A9D-94FEBD8AF56E}"/>
-    <hyperlink ref="G8" r:id="rId16" xr:uid="{7F6287CC-BB92-4E52-809C-EB767EC74917}"/>
-    <hyperlink ref="F9" r:id="rId17" xr:uid="{9D5537CD-F581-413D-8A66-80C63877287D}"/>
-    <hyperlink ref="E9" r:id="rId18" xr:uid="{077EEB8B-B00B-4029-85AA-66F6FF9F130C}"/>
-    <hyperlink ref="F10" r:id="rId19" xr:uid="{7C7FA154-6C36-4C3C-8D43-CAE0728AA7EC}"/>
-    <hyperlink ref="G13" r:id="rId20" xr:uid="{7FE86763-5FDE-4DD1-99A7-84F1E00C9A02}"/>
-    <hyperlink ref="F11" r:id="rId21" xr:uid="{D25B2287-9606-42DE-A834-84D126613B53}"/>
-    <hyperlink ref="F12" r:id="rId22" xr:uid="{478762B1-875C-42F1-93D0-68A0D6BF660E}"/>
-    <hyperlink ref="F13" r:id="rId23" xr:uid="{ABA68FFB-EB74-41DB-9588-6649333C98DD}"/>
-    <hyperlink ref="F14" r:id="rId24" xr:uid="{02F93965-893C-485F-8DD0-4C6B2DB9C6B9}"/>
-    <hyperlink ref="F15" r:id="rId25" xr:uid="{783FBFA1-A341-4EF3-96AB-0C3C7CC671CE}"/>
-    <hyperlink ref="G15" r:id="rId26" xr:uid="{E95C1D78-4D05-49BD-9223-E03DB5C01E00}"/>
-    <hyperlink ref="F16" r:id="rId27" xr:uid="{A4EA1622-5689-4860-8B97-7DB0900F171D}"/>
-    <hyperlink ref="E16" r:id="rId28" xr:uid="{7A252C51-462D-4992-9768-7BFBD4791555}"/>
-    <hyperlink ref="F17" r:id="rId29" xr:uid="{11007D7D-EB4E-4D73-8BC3-CEE2CE5EB0B3}"/>
-    <hyperlink ref="G20" r:id="rId30" xr:uid="{DA88F0B6-BA16-4080-93EC-2D9792F35A32}"/>
-    <hyperlink ref="F18" r:id="rId31" xr:uid="{28DA13AF-D189-48EE-A7BB-BF8EBD621E61}"/>
-    <hyperlink ref="F19" r:id="rId32" xr:uid="{B44C2156-177B-4280-B636-E6CBD415BC32}"/>
-    <hyperlink ref="F20" r:id="rId33" xr:uid="{37107173-85BF-4CCF-B234-416E27CF1839}"/>
-    <hyperlink ref="F21" r:id="rId34" xr:uid="{29967EB2-07F5-44FD-8D9F-1C4AC333DA99}"/>
-    <hyperlink ref="F22" r:id="rId35" xr:uid="{8275CB4D-7B85-454A-8ABA-F78A6DB6B645}"/>
-    <hyperlink ref="G22" r:id="rId36" xr:uid="{E5CAC7F5-16F0-416C-948F-075C570026B6}"/>
-    <hyperlink ref="F23" r:id="rId37" xr:uid="{14859CB8-4835-43E0-8C76-52F7FA678404}"/>
-    <hyperlink ref="F24" r:id="rId38" xr:uid="{D118EB67-B0A7-4AD9-8986-20668C4711D3}"/>
-    <hyperlink ref="G27" r:id="rId39" xr:uid="{BF46D8A2-9832-4FF9-B22A-C88B18CE5EE3}"/>
-    <hyperlink ref="F25" r:id="rId40" xr:uid="{7C978EA2-8470-4867-9E0D-449BE126D90C}"/>
-    <hyperlink ref="F26" r:id="rId41" xr:uid="{73FD11E8-D6A8-4751-87F1-22D9E3BB82ED}"/>
-    <hyperlink ref="F27" r:id="rId42" xr:uid="{188DF551-5A4F-4F16-A7DB-909AA72C9DA0}"/>
-    <hyperlink ref="F28" r:id="rId43" xr:uid="{A72AF4EF-BFA3-4023-B416-17EB87E7C301}"/>
-    <hyperlink ref="F29" r:id="rId44" xr:uid="{61130B14-8134-49FF-9794-68CA4AD3CDB9}"/>
-    <hyperlink ref="G29" r:id="rId45" xr:uid="{54400C2A-3171-469F-98E5-CBFCBF85A9F4}"/>
-    <hyperlink ref="E24" r:id="rId46" xr:uid="{3082870B-DEF9-48E1-A1E0-58B5FF41F10A}"/>
-    <hyperlink ref="E25:E30" r:id="rId47" display="U2ux5ANnR9@gmail.com" xr:uid="{5A9D4468-B949-43B4-A5D8-57F4B6F68007}"/>
-    <hyperlink ref="E10:E15" r:id="rId48" display="0HjPzxZ6l7@gmail.com" xr:uid="{C27191E6-720A-471B-B0F0-BB1978E56A88}"/>
-    <hyperlink ref="E17:E23" r:id="rId49" display="Ef0aNn38tp@gmail.com" xr:uid="{231160C3-7A7D-4CBC-B0D2-8A7B9D3E051C}"/>
+    <hyperlink ref="F41" r:id="rId1" xr:uid="{295AE882-2DF8-4C52-BCC5-272AF1488C33}"/>
+    <hyperlink ref="E41" r:id="rId2" xr:uid="{FBDF0631-83E1-4D2E-9F48-B40235C48FD0}"/>
+    <hyperlink ref="E42" r:id="rId3" xr:uid="{C70C7F0E-DA9D-43DD-8585-A8D797B68999}"/>
+    <hyperlink ref="F42" r:id="rId4" xr:uid="{8099DEDE-C1F6-482C-949B-26CD83F5AA5C}"/>
+    <hyperlink ref="G45" r:id="rId5" xr:uid="{793C0D70-8E75-4D00-A69E-9699326AEE9C}"/>
+    <hyperlink ref="E43" r:id="rId6" xr:uid="{3785A2FF-4DEE-4C1A-BF12-4A3790864C66}"/>
+    <hyperlink ref="E44" r:id="rId7" xr:uid="{3D3062FC-D8C4-468A-89F4-BAACDE63FF09}"/>
+    <hyperlink ref="E45" r:id="rId8" xr:uid="{3903EEE1-32E0-4C87-9FFC-0FFC629210D6}"/>
+    <hyperlink ref="F43" r:id="rId9" xr:uid="{32419C80-3F50-42DF-B337-2AC8C6F987AC}"/>
+    <hyperlink ref="F44" r:id="rId10" xr:uid="{8A21FEDB-B7FF-4A57-B902-E3E084BDE91F}"/>
+    <hyperlink ref="F45" r:id="rId11" xr:uid="{B6CB6B95-0774-4538-9072-07F46A5B7505}"/>
+    <hyperlink ref="E46" r:id="rId12" xr:uid="{ADF0FAE6-EB7A-4C20-BF57-BCD6EAA59F50}"/>
+    <hyperlink ref="F46" r:id="rId13" xr:uid="{E92B2622-A663-4F49-A033-F6EC6C8CC631}"/>
+    <hyperlink ref="E47" r:id="rId14" xr:uid="{5B5B3BE6-CAF4-429B-9934-7D143B88453F}"/>
+    <hyperlink ref="F47" r:id="rId15" xr:uid="{0F6B3EC9-51AA-49E0-9A9D-94FEBD8AF56E}"/>
+    <hyperlink ref="G47" r:id="rId16" xr:uid="{7F6287CC-BB92-4E52-809C-EB767EC74917}"/>
+    <hyperlink ref="F48" r:id="rId17" xr:uid="{9D5537CD-F581-413D-8A66-80C63877287D}"/>
+    <hyperlink ref="E48" r:id="rId18" xr:uid="{077EEB8B-B00B-4029-85AA-66F6FF9F130C}"/>
+    <hyperlink ref="F49" r:id="rId19" xr:uid="{7C7FA154-6C36-4C3C-8D43-CAE0728AA7EC}"/>
+    <hyperlink ref="G52" r:id="rId20" xr:uid="{7FE86763-5FDE-4DD1-99A7-84F1E00C9A02}"/>
+    <hyperlink ref="F50" r:id="rId21" xr:uid="{D25B2287-9606-42DE-A834-84D126613B53}"/>
+    <hyperlink ref="F51" r:id="rId22" xr:uid="{478762B1-875C-42F1-93D0-68A0D6BF660E}"/>
+    <hyperlink ref="F52" r:id="rId23" xr:uid="{ABA68FFB-EB74-41DB-9588-6649333C98DD}"/>
+    <hyperlink ref="F53" r:id="rId24" xr:uid="{02F93965-893C-485F-8DD0-4C6B2DB9C6B9}"/>
+    <hyperlink ref="F54" r:id="rId25" xr:uid="{783FBFA1-A341-4EF3-96AB-0C3C7CC671CE}"/>
+    <hyperlink ref="G54" r:id="rId26" xr:uid="{E95C1D78-4D05-49BD-9223-E03DB5C01E00}"/>
+    <hyperlink ref="F55" r:id="rId27" xr:uid="{A4EA1622-5689-4860-8B97-7DB0900F171D}"/>
+    <hyperlink ref="E55" r:id="rId28" xr:uid="{7A252C51-462D-4992-9768-7BFBD4791555}"/>
+    <hyperlink ref="F56" r:id="rId29" xr:uid="{11007D7D-EB4E-4D73-8BC3-CEE2CE5EB0B3}"/>
+    <hyperlink ref="G59" r:id="rId30" xr:uid="{DA88F0B6-BA16-4080-93EC-2D9792F35A32}"/>
+    <hyperlink ref="F57" r:id="rId31" xr:uid="{28DA13AF-D189-48EE-A7BB-BF8EBD621E61}"/>
+    <hyperlink ref="F58" r:id="rId32" xr:uid="{B44C2156-177B-4280-B636-E6CBD415BC32}"/>
+    <hyperlink ref="F59" r:id="rId33" xr:uid="{37107173-85BF-4CCF-B234-416E27CF1839}"/>
+    <hyperlink ref="F60" r:id="rId34" xr:uid="{29967EB2-07F5-44FD-8D9F-1C4AC333DA99}"/>
+    <hyperlink ref="F61" r:id="rId35" xr:uid="{8275CB4D-7B85-454A-8ABA-F78A6DB6B645}"/>
+    <hyperlink ref="G61" r:id="rId36" xr:uid="{E5CAC7F5-16F0-416C-948F-075C570026B6}"/>
+    <hyperlink ref="F62" r:id="rId37" xr:uid="{14859CB8-4835-43E0-8C76-52F7FA678404}"/>
+    <hyperlink ref="F63" r:id="rId38" xr:uid="{D118EB67-B0A7-4AD9-8986-20668C4711D3}"/>
+    <hyperlink ref="G66" r:id="rId39" xr:uid="{BF46D8A2-9832-4FF9-B22A-C88B18CE5EE3}"/>
+    <hyperlink ref="F64" r:id="rId40" xr:uid="{7C978EA2-8470-4867-9E0D-449BE126D90C}"/>
+    <hyperlink ref="F65" r:id="rId41" xr:uid="{73FD11E8-D6A8-4751-87F1-22D9E3BB82ED}"/>
+    <hyperlink ref="F66" r:id="rId42" xr:uid="{188DF551-5A4F-4F16-A7DB-909AA72C9DA0}"/>
+    <hyperlink ref="F67" r:id="rId43" xr:uid="{A72AF4EF-BFA3-4023-B416-17EB87E7C301}"/>
+    <hyperlink ref="F68" r:id="rId44" xr:uid="{61130B14-8134-49FF-9794-68CA4AD3CDB9}"/>
+    <hyperlink ref="G68" r:id="rId45" xr:uid="{54400C2A-3171-469F-98E5-CBFCBF85A9F4}"/>
+    <hyperlink ref="E63" r:id="rId46" xr:uid="{3082870B-DEF9-48E1-A1E0-58B5FF41F10A}"/>
+    <hyperlink ref="E64:E68" r:id="rId47" display="U2ux5ANnR9@gmail.com" xr:uid="{5A9D4468-B949-43B4-A5D8-57F4B6F68007}"/>
+    <hyperlink ref="E49:E54" r:id="rId48" display="0HjPzxZ6l7@gmail.com" xr:uid="{C27191E6-720A-471B-B0F0-BB1978E56A88}"/>
+    <hyperlink ref="E56:E62" r:id="rId49" display="Ef0aNn38tp@gmail.com" xr:uid="{231160C3-7A7D-4CBC-B0D2-8A7B9D3E051C}"/>
+    <hyperlink ref="E2" r:id="rId50" xr:uid="{FB621748-1CD6-40A1-95C3-1343F6120A0F}"/>
+    <hyperlink ref="F2" r:id="rId51" xr:uid="{B648A064-D610-415F-8F8F-1809DCAF789A}"/>
+    <hyperlink ref="E3" r:id="rId52" xr:uid="{50CEF0D1-9128-41BD-949D-535A9A23361A}"/>
+    <hyperlink ref="E4" r:id="rId53" xr:uid="{FDB21D58-4353-4ED6-B1D0-5CAAF4B0E473}"/>
+    <hyperlink ref="E5" r:id="rId54" xr:uid="{969251C1-91E1-410E-B4A5-34D9273DBCA1}"/>
+    <hyperlink ref="F3" r:id="rId55" xr:uid="{8B77DEF6-03F9-4B24-B25E-34B3D3107D33}"/>
+    <hyperlink ref="F4" r:id="rId56" xr:uid="{AE3CFF6C-11A4-4BEF-B7F8-4C6733374F76}"/>
+    <hyperlink ref="F5" r:id="rId57" xr:uid="{20AC22EF-833E-49AC-B9D4-41AA10BDA9D7}"/>
+    <hyperlink ref="E6" r:id="rId58" xr:uid="{09C049BF-83D5-45EE-9DF8-B1676A510BF8}"/>
+    <hyperlink ref="E7" r:id="rId59" xr:uid="{FD8F74EE-652E-4864-82F3-0DD70D8B589A}"/>
+    <hyperlink ref="F6" r:id="rId60" xr:uid="{9BB851C6-500D-4843-9598-C8120C6B9314}"/>
+    <hyperlink ref="F7" r:id="rId61" xr:uid="{E9181C42-4D68-43C3-97FD-5B6407CA1DFC}"/>
+    <hyperlink ref="E13" r:id="rId62" xr:uid="{A36CD2C4-73C5-4B36-AA30-029E8B9F501E}"/>
+    <hyperlink ref="F13" r:id="rId63" xr:uid="{70DDD06E-794B-46D7-A8A8-4F113D0410E5}"/>
+    <hyperlink ref="F14" r:id="rId64" xr:uid="{51A1F18A-2656-4E2E-B9E9-BF7E05528ADA}"/>
+    <hyperlink ref="F15" r:id="rId65" xr:uid="{AAD7981F-C8CE-4345-A1D2-5A84E4E831A5}"/>
+    <hyperlink ref="F16" r:id="rId66" xr:uid="{F1DABFDF-D9C4-4394-B7A2-8EDE471D11ED}"/>
+    <hyperlink ref="F17" r:id="rId67" xr:uid="{4890B1A2-A677-4AAA-A373-EC4D2B568739}"/>
+    <hyperlink ref="F18" r:id="rId68" xr:uid="{52E668E4-5140-4C67-82C5-7CEDDA40409A}"/>
+    <hyperlink ref="E14:E18" r:id="rId69" display="jqetgFWHup@gmail.com" xr:uid="{AD1F6B30-D4EC-4978-AC10-60BEAB249676}"/>
+    <hyperlink ref="E24" r:id="rId70" xr:uid="{2F918BD4-FA0D-4DA5-B342-08A5244742C5}"/>
+    <hyperlink ref="F24" r:id="rId71" xr:uid="{552E0AD7-757B-4B58-85F8-1432A08114E4}"/>
+    <hyperlink ref="F25" r:id="rId72" xr:uid="{80B61116-DEFB-4907-8934-FB95E0439E4C}"/>
+    <hyperlink ref="F26" r:id="rId73" xr:uid="{5B530658-A829-45FC-98FE-C5BDCA4444B1}"/>
+    <hyperlink ref="F27" r:id="rId74" xr:uid="{12CBC029-8D1B-4822-8761-0092925171FC}"/>
+    <hyperlink ref="F28" r:id="rId75" xr:uid="{D806DE75-57D0-4D24-A0C9-4E313EB1BF72}"/>
+    <hyperlink ref="F29" r:id="rId76" xr:uid="{810DB232-7803-4150-B3E0-71189F947221}"/>
+    <hyperlink ref="E25:E29" r:id="rId77" display="Ef0aNn38tp@gmail.com" xr:uid="{C8394861-B2BF-48C0-8E52-C71733D5E73F}"/>
+    <hyperlink ref="E35" r:id="rId78" xr:uid="{0C1760BD-CF77-4BB8-A67F-E3132035DEA4}"/>
+    <hyperlink ref="F35" r:id="rId79" xr:uid="{257174F8-8800-4A07-89DB-0BB5DEA9DB2D}"/>
+    <hyperlink ref="F36" r:id="rId80" xr:uid="{C8735D71-4BF2-4ACB-8BF8-D3809819FF93}"/>
+    <hyperlink ref="F37" r:id="rId81" xr:uid="{D7DB73EB-5DCC-4E7D-B348-48481FE5D646}"/>
+    <hyperlink ref="F38" r:id="rId82" xr:uid="{435DFCC0-6C8D-46CA-8A59-BAC2787FE79D}"/>
+    <hyperlink ref="F39" r:id="rId83" xr:uid="{DAFC5C27-AF6A-4CB2-ABF6-ED003B4DD0B6}"/>
+    <hyperlink ref="F40" r:id="rId84" xr:uid="{833F2098-DC6B-4718-94B2-63C057547C9E}"/>
+    <hyperlink ref="E36:E40" r:id="rId85" display="EcEtRWLQea@gmail.com" xr:uid="{3CF67FD5-7D27-47B0-A1A8-B34F34B68732}"/>
+    <hyperlink ref="E8" r:id="rId86" xr:uid="{831A48C0-0126-460B-A279-6B6E31015013}"/>
+    <hyperlink ref="F8" r:id="rId87" xr:uid="{39180389-E4D4-4783-857A-BEF107FA3747}"/>
+    <hyperlink ref="E9" r:id="rId88" xr:uid="{2C7E00A4-1760-4439-B28B-57FF393F4787}"/>
+    <hyperlink ref="F9" r:id="rId89" xr:uid="{D39A2A12-A30F-4D7C-9727-2C442235383B}"/>
+    <hyperlink ref="E10" r:id="rId90" xr:uid="{E6254032-706F-482D-955C-DAE69AB85351}"/>
+    <hyperlink ref="F10" r:id="rId91" xr:uid="{6E2836F6-E5C8-457D-8FA6-A2D8BD60E151}"/>
+    <hyperlink ref="E11" r:id="rId92" xr:uid="{E3BE4734-7709-450E-B445-B4C62A5BD53C}"/>
+    <hyperlink ref="F11" r:id="rId93" xr:uid="{283BA171-CB60-4961-B6ED-CF543CF58CD2}"/>
+    <hyperlink ref="E12" r:id="rId94" xr:uid="{8E7DF14A-305E-43F1-8815-ED9D3D805115}"/>
+    <hyperlink ref="F12" r:id="rId95" xr:uid="{A593FABF-56B8-4A82-8DE8-61981EBCF09F}"/>
+    <hyperlink ref="E19" r:id="rId96" xr:uid="{E25B55B3-A675-4D80-91BD-C911BC890386}"/>
+    <hyperlink ref="F19" r:id="rId97" xr:uid="{A12653AC-D0AF-41D2-9144-AF608AE338E4}"/>
+    <hyperlink ref="E20" r:id="rId98" xr:uid="{48A3382F-1432-4F32-AC32-EEBED7C1146B}"/>
+    <hyperlink ref="F20" r:id="rId99" xr:uid="{566E7410-150B-4A1F-A2AD-4304A6BBD6E1}"/>
+    <hyperlink ref="E21" r:id="rId100" xr:uid="{5A64A42C-8CBB-41D6-A3E3-5DFBC2DAA58E}"/>
+    <hyperlink ref="F21" r:id="rId101" xr:uid="{2985F80F-B35D-4F84-ADFB-7D199ECCBBD1}"/>
+    <hyperlink ref="E22" r:id="rId102" xr:uid="{5879F1A6-AF2C-4D0F-99A8-A40E7F397937}"/>
+    <hyperlink ref="F22" r:id="rId103" xr:uid="{67411216-E736-43F6-AE25-160A6CBCF8D7}"/>
+    <hyperlink ref="E23" r:id="rId104" xr:uid="{95469C35-1498-4E4D-965A-5E08C99190E9}"/>
+    <hyperlink ref="F23" r:id="rId105" xr:uid="{36B1678F-C9EB-4DAB-AB45-2231E3303600}"/>
+    <hyperlink ref="E30" r:id="rId106" xr:uid="{32A80FA6-C7B7-46DC-ABBF-5E6F7CF6A6FC}"/>
+    <hyperlink ref="F30" r:id="rId107" xr:uid="{D726DD44-3A38-484A-A3A8-47AB60062334}"/>
+    <hyperlink ref="E31" r:id="rId108" xr:uid="{61D3F85A-9985-4C5D-9B29-69A4D987E54A}"/>
+    <hyperlink ref="F31" r:id="rId109" xr:uid="{37725906-A3F0-4B4D-99CD-E32BDF7F4849}"/>
+    <hyperlink ref="E32" r:id="rId110" xr:uid="{4214D9CA-6806-4FBB-921E-D5B6E9FA867D}"/>
+    <hyperlink ref="F32" r:id="rId111" xr:uid="{552AD445-CB1E-4533-A48B-5FC4B4CDCF57}"/>
+    <hyperlink ref="E33" r:id="rId112" xr:uid="{DDE6B19C-E640-497A-8EB8-D1282ECF31C7}"/>
+    <hyperlink ref="F33" r:id="rId113" xr:uid="{F8904A9C-7624-4ED9-892B-9EED30E1A415}"/>
+    <hyperlink ref="E34" r:id="rId114" xr:uid="{795191B6-9EAA-4060-867B-8341A42A2834}"/>
+    <hyperlink ref="F34" r:id="rId115" xr:uid="{8D51D504-9F1C-4CC7-A855-0CA8709087F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId116"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the issues for accounting and dashboard.
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="269">
   <si>
     <t>TestName</t>
   </si>
@@ -833,6 +833,12 @@
   </si>
   <si>
     <t>TC_Accounting_ViewInvoice</t>
+  </si>
+  <si>
+    <t>TC_Accounting_ValidateStudentNotSelectedWarningMsg</t>
+  </si>
+  <si>
+    <t>Please select student</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,7 +1298,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -4333,8 +4339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7470,7 +7476,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7508,7 +7514,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7528,7 +7534,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -7568,7 +7574,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -7588,7 +7594,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -7608,7 +7614,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -7631,19 +7637,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7662,8 +7670,11 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>265</v>
       </c>
@@ -7671,7 +7682,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7683,7 +7694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -7701,13 +7712,38 @@
       </c>
       <c r="F3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included new cases for execution
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -1220,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -7639,7 +7639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -7682,7 +7682,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7702,7 +7702,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Fixed the sync issues
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="273">
   <si>
     <t>TestName</t>
   </si>
@@ -839,6 +839,18 @@
   </si>
   <si>
     <t>Please select student</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>04/02/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warning_Msg </t>
+  </si>
+  <si>
+    <t>The end date should be greater than to start date</t>
   </si>
 </sst>
 </file>
@@ -1220,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4339,8 +4351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7473,10 +7485,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7484,9 +7496,11 @@
     <col min="1" max="1" width="49.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7505,8 +7519,14 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>257</v>
       </c>
@@ -7526,7 +7546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>259</v>
       </c>
@@ -7546,7 +7566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>261</v>
       </c>
@@ -7566,7 +7586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>262</v>
       </c>
@@ -7586,7 +7606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>263</v>
       </c>
@@ -7606,7 +7626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>264</v>
       </c>
@@ -7624,6 +7644,12 @@
       </c>
       <c r="F7" t="s">
         <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H7" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -7632,6 +7658,7 @@
     <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7639,8 +7666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed few more sync issue
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -844,13 +844,13 @@
     <t>FromDate</t>
   </si>
   <si>
-    <t>04/02/2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">Warning_Msg </t>
   </si>
   <si>
     <t>The end date should be greater than to start date</t>
+  </si>
+  <si>
+    <t>04/04/2022</t>
   </si>
 </sst>
 </file>
@@ -7523,7 +7523,7 @@
         <v>269</v>
       </c>
       <c r="H1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -7646,10 +7646,10 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -7667,7 +7667,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7709,7 +7709,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Added a new script
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="275">
   <si>
     <t>TestName</t>
   </si>
@@ -851,6 +851,12 @@
   </si>
   <si>
     <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>TC_dashboard_validation_student</t>
+  </si>
+  <si>
+    <t>testqastudent@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -7485,10 +7491,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7652,13 +7658,34 @@
         <v>271</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2:E7" r:id="rId1" display="testqateacher@gmail.com"/>
     <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -7667,7 +7694,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7709,7 +7736,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Trying a work around for date entry issue
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -1238,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1330,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -7494,7 +7494,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7540,7 +7540,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7560,7 +7560,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -7580,7 +7580,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -7600,7 +7600,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -7620,7 +7620,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -7666,7 +7666,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -7693,7 +7693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
@@ -7736,7 +7736,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7756,7 +7756,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -7776,7 +7776,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
added receive payment script
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="278">
   <si>
     <t>TestName</t>
   </si>
@@ -857,6 +857,15 @@
   </si>
   <si>
     <t>testqastudent@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_Accounting_ReceivePayment</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Expected_Inv_Status</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1248,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,7 +1325,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -1330,7 +1339,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -7494,7 +7503,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7640,7 +7649,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -7691,10 +7700,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7702,10 +7711,11 @@
     <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7727,8 +7737,11 @@
       <c r="G1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>265</v>
       </c>
@@ -7736,7 +7749,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7748,7 +7761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -7768,7 +7781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -7789,6 +7802,29 @@
       </c>
       <c r="G4" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -7796,8 +7832,9 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushing receive payment script along with other fixes
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="277">
   <si>
     <t>TestName</t>
   </si>
@@ -863,9 +863,6 @@
   </si>
   <si>
     <t>Paid</t>
-  </si>
-  <si>
-    <t>Expected_Inv_Status</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1245,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,7 +1322,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -7503,7 +7500,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7549,7 +7546,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -7569,7 +7566,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -7589,7 +7586,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -7609,7 +7606,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -7629,7 +7626,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -7675,7 +7672,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -7703,7 +7700,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7737,9 +7734,7 @@
       <c r="G1" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>277</v>
-      </c>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -7769,7 +7764,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -7789,7 +7784,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -7823,7 +7818,7 @@
       <c r="F5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
my profile updates done
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mousiki_Latest\Selenium_Framework_Mousiki\excelinput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC50FF-A77D-46C5-ACE9-B6BEC9FAD48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="278">
   <si>
     <t>TestName</t>
   </si>
@@ -733,18 +734,12 @@
     <t>TC_myprofile_negativeflow_Student_6</t>
   </si>
   <si>
-    <t>EcEtRWLQea@gmail.com</t>
-  </si>
-  <si>
     <t>TC_myprofile_negativeflow_MusicSchool_7</t>
   </si>
   <si>
     <t>9458</t>
   </si>
   <si>
-    <t>TC_myprofile_negativeflow_MusicSchool_8</t>
-  </si>
-  <si>
     <t>D/M/YYYY</t>
   </si>
   <si>
@@ -772,9 +767,6 @@
     <t>TC_myprofile_negativeflow_Parent_7</t>
   </si>
   <si>
-    <t>TC_myprofile_negativeflow_Parent_8</t>
-  </si>
-  <si>
     <t>TC_myprofile_negativeflow_Parent_9</t>
   </si>
   <si>
@@ -787,9 +779,6 @@
     <t>TC_myprofile_negativeflow_Teacher_7</t>
   </si>
   <si>
-    <t>TC_myprofile_negativeflow_Teacher_8</t>
-  </si>
-  <si>
     <t>TC_myprofile_negativeflow_Teacher_9</t>
   </si>
   <si>
@@ -857,12 +846,33 @@
   </si>
   <si>
     <t>testqastudent@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_7</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_8</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_9</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_10</t>
+  </si>
+  <si>
+    <t>TC_myprofile_DOBnegativeflow_Student_11</t>
+  </si>
+  <si>
+    <t>9t4a5pAuYF@gmail.com</t>
+  </si>
+  <si>
+    <t>Date of Birth is Required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1235,11 +1245,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1302,7 +1312,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -1310,13 +1320,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -1324,13 +1334,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -1343,11 +1353,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4171,38 +4181,38 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8" display="Sgidfn345@"/>
-    <hyperlink ref="G8" r:id="rId9"/>
-    <hyperlink ref="H18" r:id="rId10"/>
-    <hyperlink ref="H19:H20" r:id="rId11" display="Sgidfn345@"/>
-    <hyperlink ref="H22" r:id="rId12"/>
-    <hyperlink ref="H23" r:id="rId13"/>
-    <hyperlink ref="H24" r:id="rId14"/>
-    <hyperlink ref="H25" r:id="rId15" display="Sgidfn345@"/>
-    <hyperlink ref="G24" r:id="rId16"/>
-    <hyperlink ref="H34" r:id="rId17"/>
-    <hyperlink ref="H35:H36" r:id="rId18" display="Sgidfn345@"/>
-    <hyperlink ref="H38" r:id="rId19"/>
-    <hyperlink ref="H39" r:id="rId20"/>
-    <hyperlink ref="H40" r:id="rId21"/>
-    <hyperlink ref="H41" r:id="rId22" display="Sgidfn345@"/>
-    <hyperlink ref="G40" r:id="rId23"/>
-    <hyperlink ref="H50" r:id="rId24"/>
-    <hyperlink ref="H51:H52" r:id="rId25" display="Sgidfn345@"/>
-    <hyperlink ref="H54" r:id="rId26"/>
-    <hyperlink ref="H55" r:id="rId27"/>
-    <hyperlink ref="H56" r:id="rId28"/>
-    <hyperlink ref="H57" r:id="rId29" display="Sgidfn345@"/>
-    <hyperlink ref="G56" r:id="rId30"/>
-    <hyperlink ref="H66" r:id="rId31"/>
-    <hyperlink ref="H67:H68" r:id="rId32" display="Sgidfn345@"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="H9" r:id="rId8" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="G8" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="H18" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="H19:H20" r:id="rId11" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="H22" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="H23" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="H24" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="H25" r:id="rId15" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="G24" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="H34" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="H35:H36" r:id="rId18" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="H38" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="H39" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="H40" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="H41" r:id="rId22" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="G40" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="H50" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="H51:H52" r:id="rId25" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="H54" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="H55" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="H56" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="H57" r:id="rId29" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G56" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="H66" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="H67:H68" r:id="rId32" display="Sgidfn345@" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>
@@ -4210,7 +4220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4340,13 +4350,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -4354,11 +4364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C2:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4778,7 +4788,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -4797,7 +4807,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I8" t="s">
         <v>156</v>
@@ -4809,7 +4819,7 @@
         <v>11</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>13</v>
@@ -4835,7 +4845,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
         <v>54</v>
@@ -4854,11 +4864,9 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>214</v>
-      </c>
-      <c r="I9" t="s">
-        <v>156</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I9" s="1"/>
       <c r="J9" t="s">
         <v>157</v>
       </c>
@@ -4869,7 +4877,7 @@
         <v>12</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="N9" t="s">
         <v>197</v>
@@ -4892,7 +4900,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
@@ -4911,12 +4919,12 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>241</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" t="s">
-        <v>157</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="I10" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" s="1"/>
       <c r="K10" t="s">
         <v>11</v>
       </c>
@@ -4947,7 +4955,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
@@ -4959,19 +4967,21 @@
         <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="I11" t="s">
-        <v>156</v>
-      </c>
-      <c r="J11" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>157</v>
+      </c>
       <c r="K11" t="s">
         <v>11</v>
       </c>
@@ -5002,7 +5012,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -5014,20 +5024,20 @@
         <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="I12" t="s">
         <v>156</v>
       </c>
       <c r="J12" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
         <v>11</v>
@@ -5059,7 +5069,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
@@ -5081,7 +5091,7 @@
         <v>212</v>
       </c>
       <c r="I13" t="s">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="J13" t="s">
         <v>157</v>
@@ -5116,7 +5126,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
@@ -5141,7 +5151,7 @@
         <v>156</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>208</v>
       </c>
       <c r="K14" t="s">
         <v>11</v>
@@ -5173,7 +5183,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
@@ -5192,10 +5202,10 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I15" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="J15" t="s">
         <v>157</v>
@@ -5230,7 +5240,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
@@ -5249,13 +5259,13 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I16" t="s">
         <v>156</v>
       </c>
       <c r="J16" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K16" t="s">
         <v>11</v>
@@ -5287,7 +5297,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
@@ -5306,10 +5316,10 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="I17" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="J17" t="s">
         <v>157</v>
@@ -5318,7 +5328,7 @@
         <v>11</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>13</v>
@@ -5344,7 +5354,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
@@ -5363,13 +5373,11 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>214</v>
-      </c>
-      <c r="I18" t="s">
-        <v>156</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I18" s="1"/>
       <c r="J18" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="K18" t="s">
         <v>11</v>
@@ -5413,26 +5421,24 @@
         <v>54</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="I19" t="s">
         <v>156</v>
       </c>
-      <c r="J19" t="s">
-        <v>157</v>
-      </c>
+      <c r="J19" s="1"/>
       <c r="K19" t="s">
         <v>11</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>13</v>
@@ -5458,7 +5464,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
@@ -5470,17 +5476,17 @@
         <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I20" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
         <v>157</v>
@@ -5492,7 +5498,7 @@
         <v>12</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="N20" t="s">
         <v>197</v>
@@ -5515,7 +5521,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
@@ -5527,18 +5533,20 @@
         <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>241</v>
-      </c>
-      <c r="I21" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="I21" t="s">
+        <v>156</v>
+      </c>
       <c r="J21" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
         <v>11</v>
@@ -5570,7 +5578,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
         <v>54</v>
@@ -5582,19 +5590,21 @@
         <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="I22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J22" s="1"/>
+        <v>207</v>
+      </c>
+      <c r="J22" t="s">
+        <v>157</v>
+      </c>
       <c r="K22" t="s">
         <v>11</v>
       </c>
@@ -5625,7 +5635,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
@@ -5637,20 +5647,20 @@
         <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="I23" t="s">
         <v>156</v>
       </c>
       <c r="J23" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
@@ -5682,7 +5692,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -5701,10 +5711,10 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I24" t="s">
-        <v>30</v>
+        <v>211</v>
       </c>
       <c r="J24" t="s">
         <v>157</v>
@@ -5739,7 +5749,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -5758,13 +5768,13 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I25" t="s">
         <v>156</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>211</v>
       </c>
       <c r="K25" t="s">
         <v>11</v>
@@ -5796,7 +5806,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
@@ -5808,17 +5818,17 @@
         <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="I26" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="J26" t="s">
         <v>157</v>
@@ -5827,7 +5837,7 @@
         <v>11</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>13</v>
@@ -5853,7 +5863,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="B27" t="s">
         <v>54</v>
@@ -5865,20 +5875,18 @@
         <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>212</v>
-      </c>
-      <c r="I27" t="s">
-        <v>156</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I27" s="1"/>
       <c r="J27" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="K27" t="s">
         <v>11</v>
@@ -5910,7 +5918,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
@@ -5922,21 +5930,19 @@
         <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="I28" t="s">
-        <v>211</v>
-      </c>
-      <c r="J28" t="s">
-        <v>157</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="J28" s="1"/>
       <c r="K28" t="s">
         <v>11</v>
       </c>
@@ -5967,7 +5973,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -5979,20 +5985,20 @@
         <v>54</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="J29" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="K29" t="s">
         <v>11</v>
@@ -6024,7 +6030,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
@@ -6036,26 +6042,26 @@
         <v>54</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="I30" t="s">
         <v>156</v>
       </c>
       <c r="J30" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="K30" t="s">
         <v>11</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>13</v>
@@ -6081,7 +6087,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
         <v>54</v>
@@ -6093,17 +6099,17 @@
         <v>54</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="J31" t="s">
         <v>157</v>
@@ -6115,7 +6121,7 @@
         <v>12</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="N31" t="s">
         <v>197</v>
@@ -6138,7 +6144,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="B32" t="s">
         <v>54</v>
@@ -6150,18 +6156,20 @@
         <v>54</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>241</v>
-      </c>
-      <c r="I32" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="I32" t="s">
+        <v>156</v>
+      </c>
       <c r="J32" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="K32" t="s">
         <v>11</v>
@@ -6193,7 +6201,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="B33" t="s">
         <v>54</v>
@@ -6205,19 +6213,21 @@
         <v>54</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="I33" t="s">
-        <v>156</v>
-      </c>
-      <c r="J33" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="J33" t="s">
+        <v>157</v>
+      </c>
       <c r="K33" t="s">
         <v>11</v>
       </c>
@@ -6248,7 +6258,7 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
@@ -6260,20 +6270,20 @@
         <v>54</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="I34" t="s">
         <v>156</v>
       </c>
       <c r="J34" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
       <c r="K34" t="s">
         <v>11</v>
@@ -6305,29 +6315,29 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>227</v>
+        <v>271</v>
       </c>
       <c r="B35" t="s">
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
         <v>54</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>233</v>
+        <v>276</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="I35" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="J35" t="s">
         <v>157</v>
@@ -6336,7 +6346,7 @@
         <v>11</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>13</v>
@@ -6362,32 +6372,32 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>228</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>233</v>
+        <v>276</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>212</v>
+        <v>277</v>
       </c>
       <c r="I36" t="s">
         <v>156</v>
       </c>
       <c r="J36" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="K36" t="s">
         <v>11</v>
@@ -6396,7 +6406,7 @@
         <v>12</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>13</v>
+        <v>235</v>
       </c>
       <c r="N36" t="s">
         <v>197</v>
@@ -6419,30 +6429,28 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>229</v>
+        <v>273</v>
       </c>
       <c r="B37" t="s">
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
         <v>54</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>233</v>
+        <v>276</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>212</v>
-      </c>
-      <c r="I37" t="s">
-        <v>207</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I37" s="1"/>
       <c r="J37" t="s">
         <v>157</v>
       </c>
@@ -6476,33 +6484,31 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>274</v>
       </c>
       <c r="B38" t="s">
         <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>233</v>
+        <v>276</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="I38" t="s">
         <v>156</v>
       </c>
-      <c r="J38" t="s">
-        <v>208</v>
-      </c>
+      <c r="J38" s="1"/>
       <c r="K38" t="s">
         <v>11</v>
       </c>
@@ -6533,7 +6539,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
         <v>54</v>
@@ -6545,17 +6551,17 @@
         <v>54</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="I39" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="J39" t="s">
         <v>157</v>
@@ -6590,7 +6596,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
@@ -6602,20 +6608,20 @@
         <v>54</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="I40" t="s">
         <v>156</v>
       </c>
       <c r="J40" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="K40" t="s">
         <v>11</v>
@@ -6647,7 +6653,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="B41" t="s">
         <v>54</v>
@@ -6659,19 +6665,52 @@
         <v>54</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>242</v>
+      </c>
+      <c r="I41" t="s">
+        <v>156</v>
+      </c>
+      <c r="J41" t="s">
+        <v>157</v>
+      </c>
+      <c r="K41" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N41" t="s">
+        <v>197</v>
+      </c>
+      <c r="O41" t="s">
+        <v>198</v>
+      </c>
+      <c r="P41" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R41" t="s">
+        <v>201</v>
+      </c>
+      <c r="S41" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
@@ -6683,21 +6722,52 @@
         <v>54</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>138</v>
+        <v>276</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G42" t="s">
-        <v>144</v>
-      </c>
+      <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>145</v>
+        <v>242</v>
+      </c>
+      <c r="I42" t="s">
+        <v>156</v>
+      </c>
+      <c r="J42" t="s">
+        <v>157</v>
+      </c>
+      <c r="K42" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N42" t="s">
+        <v>197</v>
+      </c>
+      <c r="O42" t="s">
+        <v>198</v>
+      </c>
+      <c r="P42" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R42" t="s">
+        <v>201</v>
+      </c>
+      <c r="S42" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
@@ -6714,16 +6784,14 @@
       <c r="F43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
@@ -6741,15 +6809,15 @@
         <v>6</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H44" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
@@ -6766,16 +6834,16 @@
       <c r="F45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>150</v>
+      <c r="G45" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H45" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
@@ -6793,15 +6861,15 @@
         <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
         <v>54</v>
@@ -6819,15 +6887,15 @@
         <v>6</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H47" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
         <v>54</v>
@@ -6839,19 +6907,21 @@
         <v>54</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" t="s">
+        <v>153</v>
+      </c>
       <c r="H48" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
@@ -6863,21 +6933,21 @@
         <v>54</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G49" t="s">
-        <v>144</v>
+      <c r="G49" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H49" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B50" t="s">
         <v>54</v>
@@ -6894,16 +6964,14 @@
       <c r="F50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
         <v>54</v>
@@ -6921,15 +6989,15 @@
         <v>6</v>
       </c>
       <c r="G51" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H51" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
         <v>54</v>
@@ -6946,16 +7014,16 @@
       <c r="F52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>150</v>
+      <c r="G52" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H52" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
@@ -6973,15 +7041,15 @@
         <v>6</v>
       </c>
       <c r="G53" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H53" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
@@ -6999,15 +7067,15 @@
         <v>6</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H54" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -7019,19 +7087,21 @@
         <v>54</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="G55" t="s">
+        <v>153</v>
+      </c>
       <c r="H55" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -7043,21 +7113,21 @@
         <v>54</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G56" t="s">
-        <v>144</v>
+      <c r="G56" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H56" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
         <v>54</v>
@@ -7074,16 +7144,14 @@
       <c r="F57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
         <v>54</v>
@@ -7101,15 +7169,15 @@
         <v>6</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
         <v>54</v>
@@ -7126,16 +7194,16 @@
       <c r="F59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>150</v>
+      <c r="G59" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H59" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
         <v>54</v>
@@ -7153,15 +7221,15 @@
         <v>6</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H60" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B61" t="s">
         <v>54</v>
@@ -7179,15 +7247,15 @@
         <v>6</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H61" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B62" t="s">
         <v>54</v>
@@ -7204,14 +7272,16 @@
       <c r="F62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G62" s="1"/>
+      <c r="G62" t="s">
+        <v>153</v>
+      </c>
       <c r="H62" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B63" t="s">
         <v>54</v>
@@ -7223,21 +7293,21 @@
         <v>54</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G63" t="s">
-        <v>144</v>
+      <c r="G63" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H63" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -7249,21 +7319,19 @@
         <v>54</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B65" t="s">
         <v>54</v>
@@ -7281,15 +7349,15 @@
         <v>6</v>
       </c>
       <c r="G65" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H65" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B66" t="s">
         <v>54</v>
@@ -7306,16 +7374,16 @@
       <c r="F66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>150</v>
+      <c r="G66" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H66" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B67" t="s">
         <v>54</v>
@@ -7333,15 +7401,15 @@
         <v>6</v>
       </c>
       <c r="G67" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
         <v>54</v>
@@ -7359,142 +7427,189 @@
         <v>6</v>
       </c>
       <c r="G68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H68" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" t="s">
+        <v>54</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" t="s">
+        <v>153</v>
+      </c>
+      <c r="H69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H70" t="s">
         <v>155</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F41" r:id="rId1"/>
-    <hyperlink ref="E41" r:id="rId2"/>
-    <hyperlink ref="E42" r:id="rId3"/>
-    <hyperlink ref="F42" r:id="rId4"/>
-    <hyperlink ref="G45" r:id="rId5"/>
-    <hyperlink ref="E43" r:id="rId6"/>
-    <hyperlink ref="E44" r:id="rId7"/>
-    <hyperlink ref="E45" r:id="rId8"/>
-    <hyperlink ref="F43" r:id="rId9"/>
-    <hyperlink ref="F44" r:id="rId10"/>
-    <hyperlink ref="F45" r:id="rId11"/>
-    <hyperlink ref="E46" r:id="rId12"/>
-    <hyperlink ref="F46" r:id="rId13"/>
-    <hyperlink ref="E47" r:id="rId14"/>
-    <hyperlink ref="F47" r:id="rId15"/>
-    <hyperlink ref="G47" r:id="rId16"/>
-    <hyperlink ref="F48" r:id="rId17"/>
-    <hyperlink ref="E48" r:id="rId18"/>
-    <hyperlink ref="F49" r:id="rId19"/>
-    <hyperlink ref="G52" r:id="rId20"/>
-    <hyperlink ref="F50" r:id="rId21"/>
-    <hyperlink ref="F51" r:id="rId22"/>
-    <hyperlink ref="F52" r:id="rId23"/>
-    <hyperlink ref="F53" r:id="rId24"/>
-    <hyperlink ref="F54" r:id="rId25"/>
-    <hyperlink ref="G54" r:id="rId26"/>
-    <hyperlink ref="F55" r:id="rId27"/>
-    <hyperlink ref="E55" r:id="rId28"/>
-    <hyperlink ref="F56" r:id="rId29"/>
-    <hyperlink ref="G59" r:id="rId30"/>
-    <hyperlink ref="F57" r:id="rId31"/>
-    <hyperlink ref="F58" r:id="rId32"/>
-    <hyperlink ref="F59" r:id="rId33"/>
-    <hyperlink ref="F60" r:id="rId34"/>
-    <hyperlink ref="F61" r:id="rId35"/>
-    <hyperlink ref="G61" r:id="rId36"/>
-    <hyperlink ref="F62" r:id="rId37"/>
-    <hyperlink ref="F63" r:id="rId38"/>
-    <hyperlink ref="G66" r:id="rId39"/>
-    <hyperlink ref="F64" r:id="rId40"/>
-    <hyperlink ref="F65" r:id="rId41"/>
-    <hyperlink ref="F66" r:id="rId42"/>
-    <hyperlink ref="F67" r:id="rId43"/>
-    <hyperlink ref="F68" r:id="rId44"/>
-    <hyperlink ref="G68" r:id="rId45"/>
-    <hyperlink ref="E63" r:id="rId46"/>
-    <hyperlink ref="E64:E68" r:id="rId47" display="U2ux5ANnR9@gmail.com"/>
-    <hyperlink ref="E49:E54" r:id="rId48" display="0HjPzxZ6l7@gmail.com"/>
-    <hyperlink ref="E56:E62" r:id="rId49" display="Ef0aNn38tp@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId50"/>
-    <hyperlink ref="F2" r:id="rId51"/>
-    <hyperlink ref="E3" r:id="rId52"/>
-    <hyperlink ref="E4" r:id="rId53"/>
-    <hyperlink ref="E5" r:id="rId54"/>
-    <hyperlink ref="F3" r:id="rId55"/>
-    <hyperlink ref="F4" r:id="rId56"/>
-    <hyperlink ref="F5" r:id="rId57"/>
-    <hyperlink ref="E6" r:id="rId58"/>
-    <hyperlink ref="E7" r:id="rId59"/>
-    <hyperlink ref="F6" r:id="rId60"/>
-    <hyperlink ref="F7" r:id="rId61"/>
-    <hyperlink ref="E13" r:id="rId62"/>
-    <hyperlink ref="F13" r:id="rId63"/>
-    <hyperlink ref="F14" r:id="rId64"/>
-    <hyperlink ref="F15" r:id="rId65"/>
-    <hyperlink ref="F16" r:id="rId66"/>
-    <hyperlink ref="F17" r:id="rId67"/>
-    <hyperlink ref="F18" r:id="rId68"/>
-    <hyperlink ref="E14:E18" r:id="rId69" display="jqetgFWHup@gmail.com"/>
-    <hyperlink ref="E24" r:id="rId70"/>
-    <hyperlink ref="F24" r:id="rId71"/>
-    <hyperlink ref="F25" r:id="rId72"/>
-    <hyperlink ref="F26" r:id="rId73"/>
-    <hyperlink ref="F27" r:id="rId74"/>
-    <hyperlink ref="F28" r:id="rId75"/>
-    <hyperlink ref="F29" r:id="rId76"/>
-    <hyperlink ref="E25:E29" r:id="rId77" display="Ef0aNn38tp@gmail.com"/>
-    <hyperlink ref="E35" r:id="rId78"/>
-    <hyperlink ref="F35" r:id="rId79"/>
-    <hyperlink ref="F36" r:id="rId80"/>
-    <hyperlink ref="F37" r:id="rId81"/>
-    <hyperlink ref="F38" r:id="rId82"/>
-    <hyperlink ref="F39" r:id="rId83"/>
-    <hyperlink ref="F40" r:id="rId84"/>
-    <hyperlink ref="E36:E40" r:id="rId85" display="EcEtRWLQea@gmail.com"/>
-    <hyperlink ref="E8" r:id="rId86"/>
-    <hyperlink ref="F8" r:id="rId87"/>
-    <hyperlink ref="E9" r:id="rId88"/>
-    <hyperlink ref="F9" r:id="rId89"/>
-    <hyperlink ref="E10" r:id="rId90"/>
-    <hyperlink ref="F10" r:id="rId91"/>
-    <hyperlink ref="E11" r:id="rId92"/>
-    <hyperlink ref="F11" r:id="rId93"/>
-    <hyperlink ref="E12" r:id="rId94"/>
-    <hyperlink ref="F12" r:id="rId95"/>
-    <hyperlink ref="E19" r:id="rId96"/>
-    <hyperlink ref="F19" r:id="rId97"/>
-    <hyperlink ref="E20" r:id="rId98"/>
-    <hyperlink ref="F20" r:id="rId99"/>
-    <hyperlink ref="E21" r:id="rId100"/>
-    <hyperlink ref="F21" r:id="rId101"/>
-    <hyperlink ref="E22" r:id="rId102"/>
-    <hyperlink ref="F22" r:id="rId103"/>
-    <hyperlink ref="E23" r:id="rId104"/>
-    <hyperlink ref="F23" r:id="rId105"/>
-    <hyperlink ref="E30" r:id="rId106"/>
-    <hyperlink ref="F30" r:id="rId107"/>
-    <hyperlink ref="E31" r:id="rId108"/>
-    <hyperlink ref="F31" r:id="rId109"/>
-    <hyperlink ref="E32" r:id="rId110"/>
-    <hyperlink ref="F32" r:id="rId111"/>
-    <hyperlink ref="E33" r:id="rId112"/>
-    <hyperlink ref="F33" r:id="rId113"/>
-    <hyperlink ref="E34" r:id="rId114"/>
-    <hyperlink ref="F34" r:id="rId115"/>
+    <hyperlink ref="F43" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E43" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E44" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F44" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="G47" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E45" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="E46" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="E47" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="F45" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="F46" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="F47" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="E48" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="F48" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="E49" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="F49" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="G49" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="F50" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="E50" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="F51" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="G54" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="F52" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="F53" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="F54" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
+    <hyperlink ref="F55" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
+    <hyperlink ref="F56" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
+    <hyperlink ref="G56" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
+    <hyperlink ref="F57" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
+    <hyperlink ref="E57" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
+    <hyperlink ref="F58" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
+    <hyperlink ref="G61" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
+    <hyperlink ref="F59" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
+    <hyperlink ref="F60" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
+    <hyperlink ref="F61" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
+    <hyperlink ref="F62" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
+    <hyperlink ref="F63" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
+    <hyperlink ref="G63" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
+    <hyperlink ref="F64" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
+    <hyperlink ref="F65" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
+    <hyperlink ref="G68" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
+    <hyperlink ref="F66" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
+    <hyperlink ref="F67" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
+    <hyperlink ref="F68" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
+    <hyperlink ref="F69" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
+    <hyperlink ref="F70" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
+    <hyperlink ref="G70" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
+    <hyperlink ref="E65" r:id="rId46" xr:uid="{00000000-0004-0000-0300-00002D000000}"/>
+    <hyperlink ref="E66:E70" r:id="rId47" display="U2ux5ANnR9@gmail.com" xr:uid="{00000000-0004-0000-0300-00002E000000}"/>
+    <hyperlink ref="E51:E56" r:id="rId48" display="0HjPzxZ6l7@gmail.com" xr:uid="{00000000-0004-0000-0300-00002F000000}"/>
+    <hyperlink ref="E58:E64" r:id="rId49" display="Ef0aNn38tp@gmail.com" xr:uid="{00000000-0004-0000-0300-000030000000}"/>
+    <hyperlink ref="E2" r:id="rId50" xr:uid="{00000000-0004-0000-0300-000031000000}"/>
+    <hyperlink ref="F2" r:id="rId51" xr:uid="{00000000-0004-0000-0300-000032000000}"/>
+    <hyperlink ref="E3" r:id="rId52" xr:uid="{00000000-0004-0000-0300-000033000000}"/>
+    <hyperlink ref="E4" r:id="rId53" xr:uid="{00000000-0004-0000-0300-000034000000}"/>
+    <hyperlink ref="E5" r:id="rId54" xr:uid="{00000000-0004-0000-0300-000035000000}"/>
+    <hyperlink ref="F3" r:id="rId55" xr:uid="{00000000-0004-0000-0300-000036000000}"/>
+    <hyperlink ref="F4" r:id="rId56" xr:uid="{00000000-0004-0000-0300-000037000000}"/>
+    <hyperlink ref="F5" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000038000000}"/>
+    <hyperlink ref="E6" r:id="rId58" xr:uid="{00000000-0004-0000-0300-000039000000}"/>
+    <hyperlink ref="E7" r:id="rId59" xr:uid="{00000000-0004-0000-0300-00003A000000}"/>
+    <hyperlink ref="F6" r:id="rId60" xr:uid="{00000000-0004-0000-0300-00003B000000}"/>
+    <hyperlink ref="F7" r:id="rId61" xr:uid="{00000000-0004-0000-0300-00003C000000}"/>
+    <hyperlink ref="F11" r:id="rId62" xr:uid="{00000000-0004-0000-0300-00003E000000}"/>
+    <hyperlink ref="F12" r:id="rId63" xr:uid="{00000000-0004-0000-0300-00003F000000}"/>
+    <hyperlink ref="F13" r:id="rId64" xr:uid="{00000000-0004-0000-0300-000040000000}"/>
+    <hyperlink ref="F14" r:id="rId65" xr:uid="{00000000-0004-0000-0300-000041000000}"/>
+    <hyperlink ref="F15" r:id="rId66" xr:uid="{00000000-0004-0000-0300-000042000000}"/>
+    <hyperlink ref="F16" r:id="rId67" xr:uid="{00000000-0004-0000-0300-000043000000}"/>
+    <hyperlink ref="E20" r:id="rId68" xr:uid="{00000000-0004-0000-0300-000045000000}"/>
+    <hyperlink ref="F20" r:id="rId69" xr:uid="{00000000-0004-0000-0300-000046000000}"/>
+    <hyperlink ref="F21" r:id="rId70" xr:uid="{00000000-0004-0000-0300-000047000000}"/>
+    <hyperlink ref="F22" r:id="rId71" xr:uid="{00000000-0004-0000-0300-000048000000}"/>
+    <hyperlink ref="F23" r:id="rId72" xr:uid="{00000000-0004-0000-0300-000049000000}"/>
+    <hyperlink ref="F24" r:id="rId73" xr:uid="{00000000-0004-0000-0300-00004A000000}"/>
+    <hyperlink ref="F25" r:id="rId74" xr:uid="{00000000-0004-0000-0300-00004B000000}"/>
+    <hyperlink ref="E21:E25" r:id="rId75" display="Ef0aNn38tp@gmail.com" xr:uid="{00000000-0004-0000-0300-00004C000000}"/>
+    <hyperlink ref="E8" r:id="rId76" xr:uid="{00000000-0004-0000-0300-000055000000}"/>
+    <hyperlink ref="F8" r:id="rId77" xr:uid="{00000000-0004-0000-0300-000056000000}"/>
+    <hyperlink ref="E9" r:id="rId78" xr:uid="{00000000-0004-0000-0300-000059000000}"/>
+    <hyperlink ref="F9" r:id="rId79" xr:uid="{00000000-0004-0000-0300-00005A000000}"/>
+    <hyperlink ref="E10" r:id="rId80" xr:uid="{00000000-0004-0000-0300-00005B000000}"/>
+    <hyperlink ref="F10" r:id="rId81" xr:uid="{00000000-0004-0000-0300-00005C000000}"/>
+    <hyperlink ref="E39" r:id="rId82" xr:uid="{00000000-0004-0000-0300-00005D000000}"/>
+    <hyperlink ref="F39" r:id="rId83" xr:uid="{00000000-0004-0000-0300-00005E000000}"/>
+    <hyperlink ref="F17" r:id="rId84" xr:uid="{00000000-0004-0000-0300-000060000000}"/>
+    <hyperlink ref="F18" r:id="rId85" xr:uid="{00000000-0004-0000-0300-000064000000}"/>
+    <hyperlink ref="F19" r:id="rId86" xr:uid="{00000000-0004-0000-0300-000066000000}"/>
+    <hyperlink ref="F40" r:id="rId87" xr:uid="{00000000-0004-0000-0300-000068000000}"/>
+    <hyperlink ref="E26" r:id="rId88" xr:uid="{00000000-0004-0000-0300-000069000000}"/>
+    <hyperlink ref="F26" r:id="rId89" xr:uid="{00000000-0004-0000-0300-00006A000000}"/>
+    <hyperlink ref="E27" r:id="rId90" xr:uid="{00000000-0004-0000-0300-00006D000000}"/>
+    <hyperlink ref="F27" r:id="rId91" xr:uid="{00000000-0004-0000-0300-00006E000000}"/>
+    <hyperlink ref="E28" r:id="rId92" xr:uid="{00000000-0004-0000-0300-00006F000000}"/>
+    <hyperlink ref="F28" r:id="rId93" xr:uid="{00000000-0004-0000-0300-000070000000}"/>
+    <hyperlink ref="E41" r:id="rId94" xr:uid="{00000000-0004-0000-0300-000071000000}"/>
+    <hyperlink ref="F41" r:id="rId95" xr:uid="{00000000-0004-0000-0300-000072000000}"/>
+    <hyperlink ref="E12:E40" r:id="rId96" display="jqetgFWHup@gmail.com" xr:uid="{643C8933-BB3B-4FC9-AF7F-015E03A81D11}"/>
+    <hyperlink ref="E11" r:id="rId97" xr:uid="{B61DE880-38BF-4FB6-A627-F3A7E0D0D9A1}"/>
+    <hyperlink ref="F29" r:id="rId98" xr:uid="{AB15B9B9-9F3E-410F-8DE0-4C33E1F601D9}"/>
+    <hyperlink ref="F30" r:id="rId99" xr:uid="{13ABAD18-A7F1-493B-A5C7-951729BC57A1}"/>
+    <hyperlink ref="F31" r:id="rId100" xr:uid="{44772269-76D1-40E7-97AC-4BC7FEEE0BE4}"/>
+    <hyperlink ref="F32" r:id="rId101" xr:uid="{41C3B6D3-0F33-442D-8A79-5B2F04E6CA62}"/>
+    <hyperlink ref="F33" r:id="rId102" xr:uid="{29AAB780-05ED-4594-A8F4-35296010A91E}"/>
+    <hyperlink ref="F34" r:id="rId103" xr:uid="{FD4FFA60-650F-4536-B90B-7344E68BCAAD}"/>
+    <hyperlink ref="F35" r:id="rId104" xr:uid="{DE76D9D3-5DAE-47E1-ACC6-92A7FCFBC81D}"/>
+    <hyperlink ref="F36" r:id="rId105" xr:uid="{9A328A91-32B0-4CB3-85C7-2894C2138A91}"/>
+    <hyperlink ref="F37" r:id="rId106" xr:uid="{C82D7809-DAB7-4BE9-A430-5110954E76A7}"/>
+    <hyperlink ref="F38" r:id="rId107" xr:uid="{594C192B-92FA-49CA-A16F-E666C6ABC8D5}"/>
+    <hyperlink ref="F42" r:id="rId108" xr:uid="{CC934970-A62C-4F3E-8EC8-E3F6007E54E2}"/>
+    <hyperlink ref="E29" r:id="rId109" xr:uid="{0835ABD4-8931-44BB-8958-01D39E4CE167}"/>
+    <hyperlink ref="E30:E42" r:id="rId110" display="9t4a5pAuYF@gmail.com" xr:uid="{258D98CF-38F2-4B84-9D87-734EC157F561}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId116"/>
+  <pageSetup orientation="portrait" r:id="rId111"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7526,15 +7641,15 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -7546,7 +7661,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -7554,7 +7669,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -7566,7 +7681,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -7574,7 +7689,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -7586,7 +7701,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -7594,7 +7709,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
@@ -7606,7 +7721,7 @@
         <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -7614,7 +7729,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -7626,7 +7741,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -7634,7 +7749,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -7646,21 +7761,21 @@
         <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -7672,7 +7787,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -7680,9 +7795,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2:E7" r:id="rId1" display="testqateacher@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E2:E7" r:id="rId1" display="testqateacher@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -7690,7 +7805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7730,7 +7845,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -7742,7 +7857,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -7750,7 +7865,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -7762,7 +7877,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -7770,7 +7885,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -7782,20 +7897,20 @@
         <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Pushing all latest fixes
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -7499,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7646,7 +7646,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -7699,7 +7699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
my profile changes updated
</commit_message>
<xml_diff>
--- a/excelinput/TestData.xlsx
+++ b/excelinput/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\app_new\Selenium_Framework_Mousiki\excelinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2220A6CF-C302-4FB8-B85C-F8EEE61B7181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A0308C-A15A-43C6-A350-11377F618AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBase" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="278">
   <si>
     <t>TestName</t>
   </si>
@@ -734,18 +734,12 @@
     <t>TC_myprofile_negativeflow_Student_6</t>
   </si>
   <si>
-    <t>EcEtRWLQea@gmail.com</t>
-  </si>
-  <si>
     <t>TC_myprofile_negativeflow_MusicSchool_7</t>
   </si>
   <si>
     <t>9458</t>
   </si>
   <si>
-    <t>TC_myprofile_negativeflow_MusicSchool_8</t>
-  </si>
-  <si>
     <t>D/M/YYYY</t>
   </si>
   <si>
@@ -773,9 +767,6 @@
     <t>TC_myprofile_negativeflow_Parent_7</t>
   </si>
   <si>
-    <t>TC_myprofile_negativeflow_Parent_8</t>
-  </si>
-  <si>
     <t>TC_myprofile_negativeflow_Parent_9</t>
   </si>
   <si>
@@ -788,9 +779,6 @@
     <t>TC_myprofile_negativeflow_Teacher_7</t>
   </si>
   <si>
-    <t>TC_myprofile_negativeflow_Teacher_8</t>
-  </si>
-  <si>
     <t>TC_myprofile_negativeflow_Teacher_9</t>
   </si>
   <si>
@@ -858,6 +846,27 @@
   </si>
   <si>
     <t>testqastudent@gmail.com</t>
+  </si>
+  <si>
+    <t>9t4a5pAuYF@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_7</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_8</t>
+  </si>
+  <si>
+    <t>Date of Birth is Required</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_9</t>
+  </si>
+  <si>
+    <t>TC_myprofile_negativeflow_Student_10</t>
+  </si>
+  <si>
+    <t>TC_myprofile_DOBnegativeflow_Student_11</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,7 +1312,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -1311,13 +1320,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -1325,7 +1334,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -4356,10 +4365,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4779,7 +4788,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -4798,7 +4807,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I8" t="s">
         <v>156</v>
@@ -4810,7 +4819,7 @@
         <v>11</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>13</v>
@@ -4836,7 +4845,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
         <v>54</v>
@@ -4855,11 +4864,9 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>214</v>
-      </c>
-      <c r="I9" t="s">
-        <v>156</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I9" s="1"/>
       <c r="J9" t="s">
         <v>157</v>
       </c>
@@ -4870,7 +4877,7 @@
         <v>12</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="N9" t="s">
         <v>197</v>
@@ -4893,7 +4900,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
@@ -4912,12 +4919,12 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>241</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" t="s">
-        <v>157</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="I10" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" s="1"/>
       <c r="K10" t="s">
         <v>11</v>
       </c>
@@ -4948,7 +4955,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
@@ -4960,19 +4967,21 @@
         <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="I11" t="s">
-        <v>156</v>
-      </c>
-      <c r="J11" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>157</v>
+      </c>
       <c r="K11" t="s">
         <v>11</v>
       </c>
@@ -5003,7 +5012,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -5015,20 +5024,20 @@
         <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="I12" t="s">
         <v>156</v>
       </c>
       <c r="J12" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
         <v>11</v>
@@ -5060,7 +5069,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
@@ -5082,7 +5091,7 @@
         <v>212</v>
       </c>
       <c r="I13" t="s">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="J13" t="s">
         <v>157</v>
@@ -5117,7 +5126,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
@@ -5142,7 +5151,7 @@
         <v>156</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>208</v>
       </c>
       <c r="K14" t="s">
         <v>11</v>
@@ -5174,7 +5183,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
@@ -5193,10 +5202,10 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I15" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="J15" t="s">
         <v>157</v>
@@ -5231,7 +5240,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
@@ -5250,13 +5259,13 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I16" t="s">
         <v>156</v>
       </c>
       <c r="J16" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K16" t="s">
         <v>11</v>
@@ -5288,7 +5297,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
@@ -5307,10 +5316,10 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="I17" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="J17" t="s">
         <v>157</v>
@@ -5319,7 +5328,7 @@
         <v>11</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>13</v>
@@ -5345,7 +5354,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
@@ -5364,13 +5373,11 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>214</v>
-      </c>
-      <c r="I18" t="s">
-        <v>156</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I18" s="1"/>
       <c r="J18" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="K18" t="s">
         <v>11</v>
@@ -5414,26 +5421,24 @@
         <v>54</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="I19" t="s">
         <v>156</v>
       </c>
-      <c r="J19" t="s">
-        <v>157</v>
-      </c>
+      <c r="J19" s="1"/>
       <c r="K19" t="s">
         <v>11</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>13</v>
@@ -5459,7 +5464,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
@@ -5471,17 +5476,17 @@
         <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I20" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
         <v>157</v>
@@ -5493,7 +5498,7 @@
         <v>12</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="N20" t="s">
         <v>197</v>
@@ -5516,7 +5521,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
@@ -5528,18 +5533,20 @@
         <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>241</v>
-      </c>
-      <c r="I21" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="I21" t="s">
+        <v>156</v>
+      </c>
       <c r="J21" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
         <v>11</v>
@@ -5571,7 +5578,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
         <v>54</v>
@@ -5583,19 +5590,21 @@
         <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="I22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J22" s="1"/>
+        <v>207</v>
+      </c>
+      <c r="J22" t="s">
+        <v>157</v>
+      </c>
       <c r="K22" t="s">
         <v>11</v>
       </c>
@@ -5626,7 +5635,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
@@ -5638,20 +5647,20 @@
         <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="I23" t="s">
         <v>156</v>
       </c>
       <c r="J23" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
@@ -5683,7 +5692,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -5702,10 +5711,10 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I24" t="s">
-        <v>30</v>
+        <v>211</v>
       </c>
       <c r="J24" t="s">
         <v>157</v>
@@ -5740,7 +5749,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -5759,13 +5768,13 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I25" t="s">
         <v>156</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>211</v>
       </c>
       <c r="K25" t="s">
         <v>11</v>
@@ -5797,7 +5806,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
@@ -5809,17 +5818,17 @@
         <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="I26" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="J26" t="s">
         <v>157</v>
@@ -5828,7 +5837,7 @@
         <v>11</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>13</v>
@@ -5854,7 +5863,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="B27" t="s">
         <v>54</v>
@@ -5866,20 +5875,18 @@
         <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>212</v>
-      </c>
-      <c r="I27" t="s">
-        <v>156</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I27" s="1"/>
       <c r="J27" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="K27" t="s">
         <v>11</v>
@@ -5911,7 +5918,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
@@ -5923,21 +5930,19 @@
         <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="I28" t="s">
-        <v>211</v>
-      </c>
-      <c r="J28" t="s">
-        <v>157</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="J28" s="1"/>
       <c r="K28" t="s">
         <v>11</v>
       </c>
@@ -5968,7 +5973,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -5980,20 +5985,20 @@
         <v>54</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>195</v>
+        <v>271</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="J29" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="K29" t="s">
         <v>11</v>
@@ -6025,7 +6030,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
@@ -6037,26 +6042,26 @@
         <v>54</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>139</v>
+        <v>271</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="I30" t="s">
         <v>156</v>
       </c>
       <c r="J30" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="K30" t="s">
         <v>11</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>13</v>
@@ -6082,7 +6087,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
         <v>54</v>
@@ -6094,17 +6099,17 @@
         <v>54</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>139</v>
+        <v>271</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="J31" t="s">
         <v>157</v>
@@ -6116,7 +6121,7 @@
         <v>12</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="N31" t="s">
         <v>197</v>
@@ -6139,7 +6144,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="B32" t="s">
         <v>54</v>
@@ -6151,18 +6156,20 @@
         <v>54</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>139</v>
+        <v>271</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>241</v>
-      </c>
-      <c r="I32" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="I32" t="s">
+        <v>156</v>
+      </c>
       <c r="J32" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="K32" t="s">
         <v>11</v>
@@ -6194,7 +6201,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="B33" t="s">
         <v>54</v>
@@ -6206,19 +6213,21 @@
         <v>54</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>139</v>
+        <v>271</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="I33" t="s">
-        <v>156</v>
-      </c>
-      <c r="J33" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="J33" t="s">
+        <v>157</v>
+      </c>
       <c r="K33" t="s">
         <v>11</v>
       </c>
@@ -6249,7 +6258,7 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
@@ -6261,20 +6270,20 @@
         <v>54</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>139</v>
+        <v>271</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="I34" t="s">
         <v>156</v>
       </c>
       <c r="J34" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
       <c r="K34" t="s">
         <v>11</v>
@@ -6306,29 +6315,29 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>227</v>
+        <v>272</v>
       </c>
       <c r="B35" t="s">
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
         <v>54</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="I35" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="J35" t="s">
         <v>157</v>
@@ -6337,7 +6346,7 @@
         <v>11</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>13</v>
@@ -6363,32 +6372,32 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="I36" t="s">
         <v>156</v>
       </c>
       <c r="J36" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="K36" t="s">
         <v>11</v>
@@ -6397,7 +6406,7 @@
         <v>12</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>13</v>
+        <v>235</v>
       </c>
       <c r="N36" t="s">
         <v>197</v>
@@ -6420,30 +6429,28 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
       <c r="B37" t="s">
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
         <v>54</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>212</v>
-      </c>
-      <c r="I37" t="s">
-        <v>207</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="I37" s="1"/>
       <c r="J37" t="s">
         <v>157</v>
       </c>
@@ -6477,33 +6484,31 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s">
         <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="I38" t="s">
         <v>156</v>
       </c>
-      <c r="J38" t="s">
-        <v>208</v>
-      </c>
+      <c r="J38" s="1"/>
       <c r="K38" t="s">
         <v>11</v>
       </c>
@@ -6534,7 +6539,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
         <v>54</v>
@@ -6546,17 +6551,17 @@
         <v>54</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="I39" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="J39" t="s">
         <v>157</v>
@@ -6591,7 +6596,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
@@ -6603,20 +6608,20 @@
         <v>54</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="I40" t="s">
         <v>156</v>
       </c>
       <c r="J40" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="K40" t="s">
         <v>11</v>
@@ -6648,7 +6653,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="B41" t="s">
         <v>54</v>
@@ -6660,19 +6665,52 @@
         <v>54</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>242</v>
+      </c>
+      <c r="I41" t="s">
+        <v>156</v>
+      </c>
+      <c r="J41" t="s">
+        <v>157</v>
+      </c>
+      <c r="K41" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N41" t="s">
+        <v>197</v>
+      </c>
+      <c r="O41" t="s">
+        <v>198</v>
+      </c>
+      <c r="P41" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R41" t="s">
+        <v>201</v>
+      </c>
+      <c r="S41" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>277</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
@@ -6684,21 +6722,52 @@
         <v>54</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>138</v>
+        <v>271</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G42" t="s">
-        <v>144</v>
-      </c>
+      <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>145</v>
+        <v>242</v>
+      </c>
+      <c r="I42" t="s">
+        <v>156</v>
+      </c>
+      <c r="J42" t="s">
+        <v>157</v>
+      </c>
+      <c r="K42" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N42" t="s">
+        <v>197</v>
+      </c>
+      <c r="O42" t="s">
+        <v>198</v>
+      </c>
+      <c r="P42" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R42" t="s">
+        <v>201</v>
+      </c>
+      <c r="S42" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
@@ -6715,16 +6784,14 @@
       <c r="F43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
@@ -6742,15 +6809,15 @@
         <v>6</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H44" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
@@ -6767,16 +6834,16 @@
       <c r="F45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>150</v>
+      <c r="G45" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H45" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
@@ -6794,15 +6861,15 @@
         <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
         <v>54</v>
@@ -6820,15 +6887,15 @@
         <v>6</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H47" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
         <v>54</v>
@@ -6840,19 +6907,21 @@
         <v>54</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" t="s">
+        <v>153</v>
+      </c>
       <c r="H48" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
@@ -6864,21 +6933,21 @@
         <v>54</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G49" t="s">
-        <v>144</v>
+      <c r="G49" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H49" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B50" t="s">
         <v>54</v>
@@ -6895,16 +6964,14 @@
       <c r="F50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
         <v>54</v>
@@ -6922,15 +6989,15 @@
         <v>6</v>
       </c>
       <c r="G51" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H51" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
         <v>54</v>
@@ -6947,16 +7014,16 @@
       <c r="F52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>150</v>
+      <c r="G52" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H52" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
@@ -6974,15 +7041,15 @@
         <v>6</v>
       </c>
       <c r="G53" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H53" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
@@ -7000,15 +7067,15 @@
         <v>6</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H54" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -7020,19 +7087,21 @@
         <v>54</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="G55" t="s">
+        <v>153</v>
+      </c>
       <c r="H55" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -7044,21 +7113,21 @@
         <v>54</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G56" t="s">
-        <v>144</v>
+      <c r="G56" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H56" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
         <v>54</v>
@@ -7075,16 +7144,14 @@
       <c r="F57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
         <v>54</v>
@@ -7102,15 +7169,15 @@
         <v>6</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
         <v>54</v>
@@ -7127,16 +7194,16 @@
       <c r="F59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>150</v>
+      <c r="G59" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H59" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
         <v>54</v>
@@ -7154,15 +7221,15 @@
         <v>6</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H60" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B61" t="s">
         <v>54</v>
@@ -7180,15 +7247,15 @@
         <v>6</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H61" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B62" t="s">
         <v>54</v>
@@ -7205,14 +7272,16 @@
       <c r="F62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G62" s="1"/>
+      <c r="G62" t="s">
+        <v>153</v>
+      </c>
       <c r="H62" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B63" t="s">
         <v>54</v>
@@ -7224,21 +7293,21 @@
         <v>54</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G63" t="s">
-        <v>144</v>
+      <c r="G63" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H63" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -7250,21 +7319,19 @@
         <v>54</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>139</v>
+        <v>195</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B65" t="s">
         <v>54</v>
@@ -7282,15 +7349,15 @@
         <v>6</v>
       </c>
       <c r="G65" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H65" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B66" t="s">
         <v>54</v>
@@ -7307,16 +7374,16 @@
       <c r="F66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>150</v>
+      <c r="G66" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H66" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B67" t="s">
         <v>54</v>
@@ -7334,15 +7401,15 @@
         <v>6</v>
       </c>
       <c r="G67" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
         <v>54</v>
@@ -7360,133 +7427,180 @@
         <v>6</v>
       </c>
       <c r="G68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H68" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" t="s">
+        <v>54</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" t="s">
+        <v>153</v>
+      </c>
+      <c r="H69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H70" t="s">
         <v>155</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F41" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E41" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E42" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="F42" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="G45" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="E43" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="E44" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="E45" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="F43" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="F44" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="F45" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="E46" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="F46" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="E47" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="F47" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
-    <hyperlink ref="G47" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="F48" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
-    <hyperlink ref="E48" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
-    <hyperlink ref="F49" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
-    <hyperlink ref="G52" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
-    <hyperlink ref="F50" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
-    <hyperlink ref="F51" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
-    <hyperlink ref="F52" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
-    <hyperlink ref="F53" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
-    <hyperlink ref="F54" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
-    <hyperlink ref="G54" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
-    <hyperlink ref="F55" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
-    <hyperlink ref="E55" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
-    <hyperlink ref="F56" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
-    <hyperlink ref="G59" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
-    <hyperlink ref="F57" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
-    <hyperlink ref="F58" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
-    <hyperlink ref="F59" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
-    <hyperlink ref="F60" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
-    <hyperlink ref="F61" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
-    <hyperlink ref="G61" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
-    <hyperlink ref="F62" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
-    <hyperlink ref="F63" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
-    <hyperlink ref="G66" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
-    <hyperlink ref="F64" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
-    <hyperlink ref="F65" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
-    <hyperlink ref="F66" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
-    <hyperlink ref="F67" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
-    <hyperlink ref="F68" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
-    <hyperlink ref="G68" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
-    <hyperlink ref="E63" r:id="rId46" xr:uid="{00000000-0004-0000-0300-00002D000000}"/>
-    <hyperlink ref="E64:E68" r:id="rId47" display="U2ux5ANnR9@gmail.com" xr:uid="{00000000-0004-0000-0300-00002E000000}"/>
-    <hyperlink ref="E49:E54" r:id="rId48" display="0HjPzxZ6l7@gmail.com" xr:uid="{00000000-0004-0000-0300-00002F000000}"/>
-    <hyperlink ref="E56:E62" r:id="rId49" display="Ef0aNn38tp@gmail.com" xr:uid="{00000000-0004-0000-0300-000030000000}"/>
-    <hyperlink ref="E2" r:id="rId50" xr:uid="{00000000-0004-0000-0300-000031000000}"/>
-    <hyperlink ref="F2" r:id="rId51" xr:uid="{00000000-0004-0000-0300-000032000000}"/>
-    <hyperlink ref="E3" r:id="rId52" xr:uid="{00000000-0004-0000-0300-000033000000}"/>
-    <hyperlink ref="E4" r:id="rId53" xr:uid="{00000000-0004-0000-0300-000034000000}"/>
-    <hyperlink ref="E5" r:id="rId54" xr:uid="{00000000-0004-0000-0300-000035000000}"/>
-    <hyperlink ref="F3" r:id="rId55" xr:uid="{00000000-0004-0000-0300-000036000000}"/>
-    <hyperlink ref="F4" r:id="rId56" xr:uid="{00000000-0004-0000-0300-000037000000}"/>
-    <hyperlink ref="F5" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000038000000}"/>
-    <hyperlink ref="E6" r:id="rId58" xr:uid="{00000000-0004-0000-0300-000039000000}"/>
-    <hyperlink ref="E7" r:id="rId59" xr:uid="{00000000-0004-0000-0300-00003A000000}"/>
-    <hyperlink ref="F6" r:id="rId60" xr:uid="{00000000-0004-0000-0300-00003B000000}"/>
-    <hyperlink ref="F7" r:id="rId61" xr:uid="{00000000-0004-0000-0300-00003C000000}"/>
-    <hyperlink ref="E13" r:id="rId62" xr:uid="{00000000-0004-0000-0300-00003D000000}"/>
-    <hyperlink ref="F13" r:id="rId63" xr:uid="{00000000-0004-0000-0300-00003E000000}"/>
-    <hyperlink ref="F14" r:id="rId64" xr:uid="{00000000-0004-0000-0300-00003F000000}"/>
-    <hyperlink ref="F15" r:id="rId65" xr:uid="{00000000-0004-0000-0300-000040000000}"/>
-    <hyperlink ref="F16" r:id="rId66" xr:uid="{00000000-0004-0000-0300-000041000000}"/>
-    <hyperlink ref="F17" r:id="rId67" xr:uid="{00000000-0004-0000-0300-000042000000}"/>
-    <hyperlink ref="F18" r:id="rId68" xr:uid="{00000000-0004-0000-0300-000043000000}"/>
-    <hyperlink ref="E14:E18" r:id="rId69" display="jqetgFWHup@gmail.com" xr:uid="{00000000-0004-0000-0300-000044000000}"/>
-    <hyperlink ref="E24" r:id="rId70" xr:uid="{00000000-0004-0000-0300-000045000000}"/>
-    <hyperlink ref="F24" r:id="rId71" xr:uid="{00000000-0004-0000-0300-000046000000}"/>
-    <hyperlink ref="F25" r:id="rId72" xr:uid="{00000000-0004-0000-0300-000047000000}"/>
-    <hyperlink ref="F26" r:id="rId73" xr:uid="{00000000-0004-0000-0300-000048000000}"/>
-    <hyperlink ref="F27" r:id="rId74" xr:uid="{00000000-0004-0000-0300-000049000000}"/>
-    <hyperlink ref="F28" r:id="rId75" xr:uid="{00000000-0004-0000-0300-00004A000000}"/>
-    <hyperlink ref="F29" r:id="rId76" xr:uid="{00000000-0004-0000-0300-00004B000000}"/>
-    <hyperlink ref="E25:E29" r:id="rId77" display="Ef0aNn38tp@gmail.com" xr:uid="{00000000-0004-0000-0300-00004C000000}"/>
-    <hyperlink ref="E35" r:id="rId78" xr:uid="{00000000-0004-0000-0300-00004D000000}"/>
-    <hyperlink ref="F35" r:id="rId79" xr:uid="{00000000-0004-0000-0300-00004E000000}"/>
-    <hyperlink ref="F36" r:id="rId80" xr:uid="{00000000-0004-0000-0300-00004F000000}"/>
-    <hyperlink ref="F37" r:id="rId81" xr:uid="{00000000-0004-0000-0300-000050000000}"/>
-    <hyperlink ref="F38" r:id="rId82" xr:uid="{00000000-0004-0000-0300-000051000000}"/>
-    <hyperlink ref="F39" r:id="rId83" xr:uid="{00000000-0004-0000-0300-000052000000}"/>
-    <hyperlink ref="F40" r:id="rId84" xr:uid="{00000000-0004-0000-0300-000053000000}"/>
-    <hyperlink ref="E36:E40" r:id="rId85" display="EcEtRWLQea@gmail.com" xr:uid="{00000000-0004-0000-0300-000054000000}"/>
-    <hyperlink ref="E8" r:id="rId86" xr:uid="{00000000-0004-0000-0300-000055000000}"/>
-    <hyperlink ref="F8" r:id="rId87" xr:uid="{00000000-0004-0000-0300-000056000000}"/>
-    <hyperlink ref="E9" r:id="rId88" xr:uid="{00000000-0004-0000-0300-000057000000}"/>
-    <hyperlink ref="F9" r:id="rId89" xr:uid="{00000000-0004-0000-0300-000058000000}"/>
-    <hyperlink ref="E10" r:id="rId90" xr:uid="{00000000-0004-0000-0300-000059000000}"/>
-    <hyperlink ref="F10" r:id="rId91" xr:uid="{00000000-0004-0000-0300-00005A000000}"/>
-    <hyperlink ref="E11" r:id="rId92" xr:uid="{00000000-0004-0000-0300-00005B000000}"/>
-    <hyperlink ref="F11" r:id="rId93" xr:uid="{00000000-0004-0000-0300-00005C000000}"/>
-    <hyperlink ref="E12" r:id="rId94" xr:uid="{00000000-0004-0000-0300-00005D000000}"/>
-    <hyperlink ref="F12" r:id="rId95" xr:uid="{00000000-0004-0000-0300-00005E000000}"/>
-    <hyperlink ref="E19" r:id="rId96" xr:uid="{00000000-0004-0000-0300-00005F000000}"/>
-    <hyperlink ref="F19" r:id="rId97" xr:uid="{00000000-0004-0000-0300-000060000000}"/>
-    <hyperlink ref="E20" r:id="rId98" xr:uid="{00000000-0004-0000-0300-000061000000}"/>
-    <hyperlink ref="F20" r:id="rId99" xr:uid="{00000000-0004-0000-0300-000062000000}"/>
-    <hyperlink ref="E21" r:id="rId100" xr:uid="{00000000-0004-0000-0300-000063000000}"/>
-    <hyperlink ref="F21" r:id="rId101" xr:uid="{00000000-0004-0000-0300-000064000000}"/>
-    <hyperlink ref="E22" r:id="rId102" xr:uid="{00000000-0004-0000-0300-000065000000}"/>
-    <hyperlink ref="F22" r:id="rId103" xr:uid="{00000000-0004-0000-0300-000066000000}"/>
-    <hyperlink ref="E23" r:id="rId104" xr:uid="{00000000-0004-0000-0300-000067000000}"/>
-    <hyperlink ref="F23" r:id="rId105" xr:uid="{00000000-0004-0000-0300-000068000000}"/>
-    <hyperlink ref="E30" r:id="rId106" xr:uid="{00000000-0004-0000-0300-000069000000}"/>
-    <hyperlink ref="F30" r:id="rId107" xr:uid="{00000000-0004-0000-0300-00006A000000}"/>
-    <hyperlink ref="E31" r:id="rId108" xr:uid="{00000000-0004-0000-0300-00006B000000}"/>
-    <hyperlink ref="F31" r:id="rId109" xr:uid="{00000000-0004-0000-0300-00006C000000}"/>
-    <hyperlink ref="E32" r:id="rId110" xr:uid="{00000000-0004-0000-0300-00006D000000}"/>
-    <hyperlink ref="F32" r:id="rId111" xr:uid="{00000000-0004-0000-0300-00006E000000}"/>
-    <hyperlink ref="E33" r:id="rId112" xr:uid="{00000000-0004-0000-0300-00006F000000}"/>
-    <hyperlink ref="F33" r:id="rId113" xr:uid="{00000000-0004-0000-0300-000070000000}"/>
-    <hyperlink ref="E34" r:id="rId114" xr:uid="{00000000-0004-0000-0300-000071000000}"/>
-    <hyperlink ref="F34" r:id="rId115" xr:uid="{00000000-0004-0000-0300-000072000000}"/>
+    <hyperlink ref="F43" r:id="rId1" xr:uid="{452350F0-C67B-4EE4-9B6F-237BD8148135}"/>
+    <hyperlink ref="E43" r:id="rId2" xr:uid="{D0FBDE81-C65E-46B4-B9AD-EB159B1C0A98}"/>
+    <hyperlink ref="E44" r:id="rId3" xr:uid="{72BCBDBA-1C57-4B10-A63E-D7C55C7CE71C}"/>
+    <hyperlink ref="F44" r:id="rId4" xr:uid="{F8A1ECE0-7B00-442D-9B79-DECC5BE39035}"/>
+    <hyperlink ref="G47" r:id="rId5" xr:uid="{E9B2DB83-B7EE-4B2D-A8E8-0E9C9B94A438}"/>
+    <hyperlink ref="E45" r:id="rId6" xr:uid="{CB2BC643-B5B8-4AD8-9F47-441F181C70AD}"/>
+    <hyperlink ref="E46" r:id="rId7" xr:uid="{74BC4D4B-197B-45A2-9E4A-E516129CFF8C}"/>
+    <hyperlink ref="E47" r:id="rId8" xr:uid="{85A223A4-0043-468D-A531-26C62B36E015}"/>
+    <hyperlink ref="F45" r:id="rId9" xr:uid="{304A7452-5B5B-488A-B3F5-876887C6431B}"/>
+    <hyperlink ref="F46" r:id="rId10" xr:uid="{DC00261C-009F-4101-BEA1-14977303092D}"/>
+    <hyperlink ref="F47" r:id="rId11" xr:uid="{94BF0565-C2CD-4F39-9FA1-70160A8AD9C1}"/>
+    <hyperlink ref="E48" r:id="rId12" xr:uid="{67827A05-8D5F-4B72-B7AA-A0586D75C9DF}"/>
+    <hyperlink ref="F48" r:id="rId13" xr:uid="{F8ACDF23-8C89-4386-8F51-2F62B11123B4}"/>
+    <hyperlink ref="E49" r:id="rId14" xr:uid="{C3E18C63-2FA9-4A10-BEB0-4397F0190C77}"/>
+    <hyperlink ref="F49" r:id="rId15" xr:uid="{FFE6C54E-EDEE-4D98-A219-07EC8795B0BC}"/>
+    <hyperlink ref="G49" r:id="rId16" xr:uid="{E5A81419-DB7F-4211-A1ED-3DE503460CE9}"/>
+    <hyperlink ref="F50" r:id="rId17" xr:uid="{7E2CFDA9-DE8F-4647-9937-B8DC6968E93C}"/>
+    <hyperlink ref="E50" r:id="rId18" xr:uid="{A0322C06-D3DC-418C-ADB7-C334FA9C1C8F}"/>
+    <hyperlink ref="F51" r:id="rId19" xr:uid="{BEF24237-90B7-4B62-A3AA-AD8EC9247B5B}"/>
+    <hyperlink ref="G54" r:id="rId20" xr:uid="{C81DA955-D57A-4373-AC39-948BA95D2DBA}"/>
+    <hyperlink ref="F52" r:id="rId21" xr:uid="{3208184B-45E6-463A-B2D5-732807B4D959}"/>
+    <hyperlink ref="F53" r:id="rId22" xr:uid="{3E93F6A7-179A-4979-A2F9-23B18AF6CE76}"/>
+    <hyperlink ref="F54" r:id="rId23" xr:uid="{C7860A43-A0D2-463E-B0D1-B72797C78180}"/>
+    <hyperlink ref="F55" r:id="rId24" xr:uid="{CDD08D11-7CDD-44BF-9707-67BAD43233EB}"/>
+    <hyperlink ref="F56" r:id="rId25" xr:uid="{F1D23906-3852-4AA8-9613-52C5FAF2C8D2}"/>
+    <hyperlink ref="G56" r:id="rId26" xr:uid="{A23DB90A-2B23-4D44-ACB8-133F1E9F6105}"/>
+    <hyperlink ref="F57" r:id="rId27" xr:uid="{8C3099A6-674F-4AE8-B6D1-E424682DDDE4}"/>
+    <hyperlink ref="E57" r:id="rId28" xr:uid="{E95EF2E2-EF87-46BA-8320-A5BE68997A1C}"/>
+    <hyperlink ref="F58" r:id="rId29" xr:uid="{B490715D-7835-43EB-AA7E-FF0A53B8E0F5}"/>
+    <hyperlink ref="G61" r:id="rId30" xr:uid="{7328BC07-C04A-40BF-83D3-94B8F2FE0CA9}"/>
+    <hyperlink ref="F59" r:id="rId31" xr:uid="{2A3CD1BF-6A41-4DAB-BC20-CB790131BCD6}"/>
+    <hyperlink ref="F60" r:id="rId32" xr:uid="{F7085BE6-0D8F-478D-AAA0-8DF99AF8A99B}"/>
+    <hyperlink ref="F61" r:id="rId33" xr:uid="{B15176D3-D259-4053-B0BD-B672525CF90C}"/>
+    <hyperlink ref="F62" r:id="rId34" xr:uid="{D917340C-D58F-4475-A987-E03F24936DE4}"/>
+    <hyperlink ref="F63" r:id="rId35" xr:uid="{51A846C7-DA3E-49BE-853B-1A3B02734664}"/>
+    <hyperlink ref="G63" r:id="rId36" xr:uid="{F44651EC-567A-477F-B15E-6BFC9029869C}"/>
+    <hyperlink ref="F64" r:id="rId37" xr:uid="{A625FFAC-58C3-43A1-8C53-06BCB5317830}"/>
+    <hyperlink ref="F65" r:id="rId38" xr:uid="{67B4E9F5-F369-4B9A-BD5D-201DC3530C6A}"/>
+    <hyperlink ref="G68" r:id="rId39" xr:uid="{F893F5B8-6D5B-4290-AC1A-486DFC8289D9}"/>
+    <hyperlink ref="F66" r:id="rId40" xr:uid="{A03B509D-5421-4D52-BA10-770C5D7FAC9D}"/>
+    <hyperlink ref="F67" r:id="rId41" xr:uid="{B96CB1D0-614C-4BCA-83E3-41BCBB96D7F3}"/>
+    <hyperlink ref="F68" r:id="rId42" xr:uid="{449F2177-4F37-4D77-B80C-13941602E21E}"/>
+    <hyperlink ref="F69" r:id="rId43" xr:uid="{16E9EF77-5596-4416-A35E-5602BBF25E28}"/>
+    <hyperlink ref="F70" r:id="rId44" xr:uid="{BF8BBEC4-E359-4476-9672-C04C5CB534BC}"/>
+    <hyperlink ref="G70" r:id="rId45" xr:uid="{83E768D0-B88D-4048-BAF4-5B16D11EA180}"/>
+    <hyperlink ref="E65" r:id="rId46" xr:uid="{6710C3A0-E07D-4F2F-858D-6CAA2AAEA2C7}"/>
+    <hyperlink ref="E66:E70" r:id="rId47" display="U2ux5ANnR9@gmail.com" xr:uid="{7C043D38-0EB9-4AAF-B925-194B642A150A}"/>
+    <hyperlink ref="E51:E56" r:id="rId48" display="0HjPzxZ6l7@gmail.com" xr:uid="{9F8A6E6F-A49D-489B-A4CE-5BA4C60DD0C0}"/>
+    <hyperlink ref="E58:E64" r:id="rId49" display="Ef0aNn38tp@gmail.com" xr:uid="{FA4A8F0D-968F-41F6-B03A-695B16382166}"/>
+    <hyperlink ref="E2" r:id="rId50" xr:uid="{4149B968-9615-4BD9-8220-416955DD264D}"/>
+    <hyperlink ref="F2" r:id="rId51" xr:uid="{8314325D-9B2C-4494-BB6A-E98C233DA72F}"/>
+    <hyperlink ref="E3" r:id="rId52" xr:uid="{33E6D5FE-6B74-4FE7-98F3-09FAD1E70344}"/>
+    <hyperlink ref="E4" r:id="rId53" xr:uid="{0D949E0A-68B3-40FA-B266-6AD801893DB5}"/>
+    <hyperlink ref="E5" r:id="rId54" xr:uid="{6423E715-1471-4B8A-8B99-DA36832A06E0}"/>
+    <hyperlink ref="F3" r:id="rId55" xr:uid="{6DDD536A-A781-4D98-A801-629A28B8145A}"/>
+    <hyperlink ref="F4" r:id="rId56" xr:uid="{4293A113-E6A6-4055-A21B-53DEFBB51B29}"/>
+    <hyperlink ref="F5" r:id="rId57" xr:uid="{0653718E-9B34-46F5-AE5A-6A326209A496}"/>
+    <hyperlink ref="E6" r:id="rId58" xr:uid="{17918D8C-AD97-4301-B2AD-E7601B353B0A}"/>
+    <hyperlink ref="E7" r:id="rId59" xr:uid="{F269A10E-29ED-4119-B8AD-76770F637F0B}"/>
+    <hyperlink ref="F6" r:id="rId60" xr:uid="{D7F284AE-39BF-4644-BC71-F3C456422446}"/>
+    <hyperlink ref="F7" r:id="rId61" xr:uid="{E7F80826-A741-499C-A8A9-92C861465EA6}"/>
+    <hyperlink ref="F11" r:id="rId62" xr:uid="{034D0E6F-372E-466B-9025-03B25B8C6898}"/>
+    <hyperlink ref="F12" r:id="rId63" xr:uid="{857E1845-01A6-4CF6-BE0C-D98F7CDFADF4}"/>
+    <hyperlink ref="F13" r:id="rId64" xr:uid="{03701419-BAB1-4DEA-BDA1-C3D0A0BD0D4F}"/>
+    <hyperlink ref="F14" r:id="rId65" xr:uid="{871724FE-0C68-4EFE-B803-5C9A1CE7126F}"/>
+    <hyperlink ref="F15" r:id="rId66" xr:uid="{AB9261FE-4D44-489A-A0CD-E8323C82C687}"/>
+    <hyperlink ref="F16" r:id="rId67" xr:uid="{11BD0D6C-B989-4BFF-B307-2D5230C02456}"/>
+    <hyperlink ref="E20" r:id="rId68" xr:uid="{6BC67425-DEDC-467E-B096-525F26C8DCD0}"/>
+    <hyperlink ref="F20" r:id="rId69" xr:uid="{AEE13930-674B-4B9A-ADCF-878DD57EEFCF}"/>
+    <hyperlink ref="F21" r:id="rId70" xr:uid="{D3077800-4796-4DE5-A12A-1A74104C56E2}"/>
+    <hyperlink ref="F22" r:id="rId71" xr:uid="{F725F1B6-B6D6-43D5-8104-0D29B3608127}"/>
+    <hyperlink ref="F23" r:id="rId72" xr:uid="{E9233011-F7CF-4EDE-B669-DF6F5BDA4EDA}"/>
+    <hyperlink ref="F24" r:id="rId73" xr:uid="{0EB71D2F-3228-4751-8213-B97A682F6AC2}"/>
+    <hyperlink ref="F25" r:id="rId74" xr:uid="{9D4D9B15-6D89-41E8-ADE3-2199998FA6C7}"/>
+    <hyperlink ref="E21:E25" r:id="rId75" display="Ef0aNn38tp@gmail.com" xr:uid="{10F429A2-F58C-4B5A-8F9B-9B800386E955}"/>
+    <hyperlink ref="E8" r:id="rId76" xr:uid="{64E13DA0-F12E-4040-B878-20279A60ED0B}"/>
+    <hyperlink ref="F8" r:id="rId77" xr:uid="{5C9BDD6C-2BB7-4047-A7AE-9D1F04F38885}"/>
+    <hyperlink ref="E9" r:id="rId78" xr:uid="{D86AF3CD-FCA8-450D-96AA-032F492A7942}"/>
+    <hyperlink ref="F9" r:id="rId79" xr:uid="{C3EBA3D1-72E8-4A0C-8C92-886DAD85ECC3}"/>
+    <hyperlink ref="E10" r:id="rId80" xr:uid="{6A503D9B-4471-4DB7-BA31-8B2ED87D2FE6}"/>
+    <hyperlink ref="F10" r:id="rId81" xr:uid="{0A19E57B-4CBE-4C25-AE3A-EE528DC7100E}"/>
+    <hyperlink ref="E39" r:id="rId82" xr:uid="{CDCDE17C-74F1-4BE7-A105-E698AE77C400}"/>
+    <hyperlink ref="F39" r:id="rId83" xr:uid="{9E236A0C-4A64-47E6-B4FE-A6F21EC77B1E}"/>
+    <hyperlink ref="F17" r:id="rId84" xr:uid="{D33618A2-4380-427A-8BD5-21A20079F910}"/>
+    <hyperlink ref="F18" r:id="rId85" xr:uid="{F7840155-3F53-41A8-8014-0DD26B1EA065}"/>
+    <hyperlink ref="F19" r:id="rId86" xr:uid="{1A49A925-DC77-4530-B9EE-71B0626C6760}"/>
+    <hyperlink ref="F40" r:id="rId87" xr:uid="{ACFEA011-2582-4FCD-8CFE-2A5E4015F2F1}"/>
+    <hyperlink ref="E26" r:id="rId88" xr:uid="{C47966D3-18EC-442C-8358-16427E2F72DE}"/>
+    <hyperlink ref="F26" r:id="rId89" xr:uid="{C69FBCFD-46E3-476D-8ACB-954D28702768}"/>
+    <hyperlink ref="E27" r:id="rId90" xr:uid="{1E27FB30-19C6-4438-A67E-6D5E6BF5BF66}"/>
+    <hyperlink ref="F27" r:id="rId91" xr:uid="{7E6C81DD-0B47-4E45-9B05-393F74EC15FE}"/>
+    <hyperlink ref="E28" r:id="rId92" xr:uid="{B774DEC8-EF83-4F6D-9EA4-59FF70019EDA}"/>
+    <hyperlink ref="F28" r:id="rId93" xr:uid="{77D599A2-FEFE-496B-8552-706B4AC75DEC}"/>
+    <hyperlink ref="E41" r:id="rId94" xr:uid="{E5AC6FD2-B9B0-4D6A-A944-F1F991B8D8E9}"/>
+    <hyperlink ref="F41" r:id="rId95" xr:uid="{6E69B299-A003-47CF-A47A-E0C5A588C783}"/>
+    <hyperlink ref="E12:E40" r:id="rId96" display="jqetgFWHup@gmail.com" xr:uid="{0FB74B3B-AEDC-4265-A44F-07AE130965D1}"/>
+    <hyperlink ref="E11" r:id="rId97" xr:uid="{4564CB55-F025-42BE-950C-5387DC586EA1}"/>
+    <hyperlink ref="F29" r:id="rId98" xr:uid="{C8DA3192-F726-4F22-B238-9CA935382788}"/>
+    <hyperlink ref="F30" r:id="rId99" xr:uid="{9AEA5E85-9883-4360-A641-346D27F0EBB7}"/>
+    <hyperlink ref="F31" r:id="rId100" xr:uid="{09B97DDA-5DBF-4BAE-96AE-E3A08A9F8896}"/>
+    <hyperlink ref="F32" r:id="rId101" xr:uid="{0F549448-6962-4480-8549-1B3E3F8E55A6}"/>
+    <hyperlink ref="F33" r:id="rId102" xr:uid="{C46E2F97-9260-4FBF-9A18-D076C9EA2ACF}"/>
+    <hyperlink ref="F34" r:id="rId103" xr:uid="{14E71639-61FD-46FE-8B48-7ECC8B087942}"/>
+    <hyperlink ref="F35" r:id="rId104" xr:uid="{E3175200-01D1-4527-9F7F-4F079D801BF1}"/>
+    <hyperlink ref="F36" r:id="rId105" xr:uid="{2F8B1D8D-43A2-4D6A-B2AB-490D04C1F76B}"/>
+    <hyperlink ref="F37" r:id="rId106" xr:uid="{8617E9DF-D45D-4A61-A2BB-2B2D3BB20E4B}"/>
+    <hyperlink ref="F38" r:id="rId107" xr:uid="{1E13E3A7-3FFB-48D7-86BC-1F0AD9666B58}"/>
+    <hyperlink ref="F42" r:id="rId108" xr:uid="{F379EE4C-3F54-4A14-BDAE-BC44F49F1FB5}"/>
+    <hyperlink ref="E29" r:id="rId109" xr:uid="{5D4AC98D-1A29-4649-8C91-F5F808E09F42}"/>
+    <hyperlink ref="E30:E42" r:id="rId110" display="9t4a5pAuYF@gmail.com" xr:uid="{29E6AAB9-17B0-4409-8121-C859BE594289}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId116"/>
+  <pageSetup orientation="portrait" r:id="rId111"/>
 </worksheet>
 </file>
 
@@ -7527,15 +7641,15 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -7547,7 +7661,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -7555,7 +7669,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -7567,7 +7681,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -7575,7 +7689,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -7587,7 +7701,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -7595,7 +7709,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
@@ -7607,7 +7721,7 @@
         <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -7615,7 +7729,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -7627,7 +7741,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -7635,7 +7749,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -7647,21 +7761,21 @@
         <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -7673,7 +7787,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -7731,7 +7845,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -7743,7 +7857,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -7751,7 +7865,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -7763,7 +7877,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -7771,7 +7885,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -7783,13 +7897,13 @@
         <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>